<commit_message>
upd - cleaned mass flux file and saved it as an RDS for future use.
</commit_message>
<xml_diff>
--- a/Watershed_table_v1.xlsx
+++ b/Watershed_table_v1.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/MW/2020 Trent University/R/Thesis Data/MSc_data_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B7ABEFC-1746-694D-8120-5AEF98D00EDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59F7C266-3A6C-494F-BD3B-76605599052A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{3AD1715B-176F-3140-B9AE-F64F14EE2DEE}"/>
+    <workbookView xWindow="9600" yWindow="2300" windowWidth="28800" windowHeight="17500" xr2:uid="{3AD1715B-176F-3140-B9AE-F64F14EE2DEE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="103">
   <si>
     <t>Site name</t>
   </si>
@@ -438,7 +439,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -451,8 +452,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -521,11 +528,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -559,9 +581,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -580,6 +599,48 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -896,13 +957,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB97E4CB-EAC5-A646-BEC3-C9E17C7337B6}">
-  <dimension ref="A1:AH31"/>
+  <dimension ref="A1:AG31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="174" zoomScaleNormal="162" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="I7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L10" sqref="L10"/>
+      <selection pane="bottomRight" activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -913,7 +974,7 @@
     <col min="22" max="22" width="10.5" style="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="53" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" ht="53" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1013,9 +1074,8 @@
       <c r="AG1" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="AH1" s="13"/>
     </row>
-    <row r="2" spans="1:34" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
@@ -1064,7 +1124,7 @@
       <c r="P2" s="5">
         <v>12.43</v>
       </c>
-      <c r="Q2" s="20">
+      <c r="Q2" s="19">
         <v>2.61</v>
       </c>
       <c r="R2" s="10">
@@ -1116,7 +1176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:34" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
@@ -1165,7 +1225,7 @@
       <c r="P3" s="5">
         <v>3.61</v>
       </c>
-      <c r="Q3" s="20">
+      <c r="Q3" s="19">
         <v>0.97</v>
       </c>
       <c r="R3" s="10">
@@ -1217,7 +1277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:34" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>15</v>
       </c>
@@ -1266,7 +1326,7 @@
       <c r="P4" s="5">
         <v>3.95</v>
       </c>
-      <c r="Q4" s="20">
+      <c r="Q4" s="19">
         <v>1.46</v>
       </c>
       <c r="R4" s="10">
@@ -1318,7 +1378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:34" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>16</v>
       </c>
@@ -1367,7 +1427,7 @@
       <c r="P5" s="5">
         <v>4.8099999999999996</v>
       </c>
-      <c r="Q5" s="20">
+      <c r="Q5" s="19">
         <v>3.44</v>
       </c>
       <c r="R5" s="10">
@@ -1419,7 +1479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:34" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>17</v>
       </c>
@@ -1468,7 +1528,7 @@
       <c r="P6" s="5">
         <v>5.53</v>
       </c>
-      <c r="Q6" s="20">
+      <c r="Q6" s="19">
         <v>1.48</v>
       </c>
       <c r="R6" s="10">
@@ -1520,7 +1580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:34" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>18</v>
       </c>
@@ -1569,7 +1629,7 @@
       <c r="P7" s="5">
         <v>5.1100000000000003</v>
       </c>
-      <c r="Q7" s="20">
+      <c r="Q7" s="19">
         <v>3.87</v>
       </c>
       <c r="R7" s="10">
@@ -1621,7 +1681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:34" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>19</v>
       </c>
@@ -1670,7 +1730,7 @@
       <c r="P8" s="5">
         <v>16.91</v>
       </c>
-      <c r="Q8" s="20">
+      <c r="Q8" s="19">
         <v>14.34</v>
       </c>
       <c r="R8" s="10">
@@ -1709,7 +1769,7 @@
       <c r="AC8" s="10">
         <v>0</v>
       </c>
-      <c r="AD8" s="14">
+      <c r="AD8" s="13">
         <v>25.27</v>
       </c>
       <c r="AE8" s="10">
@@ -1722,7 +1782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:34" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
@@ -1756,13 +1816,13 @@
       <c r="K9" s="5">
         <v>7.21</v>
       </c>
-      <c r="L9" s="23">
+      <c r="L9" s="22">
         <v>11.6</v>
       </c>
-      <c r="M9" s="19">
+      <c r="M9" s="18">
         <v>4.9000000000000004</v>
       </c>
-      <c r="N9" s="21">
+      <c r="N9" s="20">
         <v>18.5</v>
       </c>
       <c r="O9" s="5">
@@ -1771,7 +1831,7 @@
       <c r="P9" s="5">
         <v>7.61</v>
       </c>
-      <c r="Q9" s="20">
+      <c r="Q9" s="19">
         <v>15.21</v>
       </c>
       <c r="R9" s="10">
@@ -1823,7 +1883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:34" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>22</v>
       </c>
@@ -1872,7 +1932,7 @@
       <c r="P10" s="5">
         <v>19.350000000000001</v>
       </c>
-      <c r="Q10" s="20">
+      <c r="Q10" s="19">
         <v>12.69</v>
       </c>
       <c r="R10" s="10">
@@ -1924,7 +1984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:34" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
@@ -1973,7 +2033,7 @@
       <c r="P11" s="5">
         <v>4.21</v>
       </c>
-      <c r="Q11" s="20">
+      <c r="Q11" s="19">
         <v>17.64</v>
       </c>
       <c r="R11" s="10">
@@ -2015,7 +2075,7 @@
       <c r="AD11" s="10">
         <v>0</v>
       </c>
-      <c r="AE11" s="15">
+      <c r="AE11" s="14">
         <v>9</v>
       </c>
       <c r="AF11" s="10">
@@ -2025,7 +2085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:34" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>25</v>
       </c>
@@ -2074,7 +2134,7 @@
       <c r="P12" s="5">
         <v>18.12</v>
       </c>
-      <c r="Q12" s="20">
+      <c r="Q12" s="19">
         <v>3.91</v>
       </c>
       <c r="R12" s="10">
@@ -2126,7 +2186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:34" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>26</v>
       </c>
@@ -2175,7 +2235,7 @@
       <c r="P13" s="5">
         <v>22.66</v>
       </c>
-      <c r="Q13" s="20">
+      <c r="Q13" s="19">
         <v>4.62</v>
       </c>
       <c r="R13" s="10">
@@ -2227,7 +2287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:34" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>27</v>
       </c>
@@ -2276,7 +2336,7 @@
       <c r="P14" s="5">
         <v>8.15</v>
       </c>
-      <c r="Q14" s="20">
+      <c r="Q14" s="19">
         <v>4.7699999999999996</v>
       </c>
       <c r="R14" s="10">
@@ -2297,7 +2357,7 @@
       <c r="W14" s="10">
         <v>0.08</v>
       </c>
-      <c r="X14" s="16">
+      <c r="X14" s="15">
         <v>0.5</v>
       </c>
       <c r="Y14" s="10">
@@ -2309,7 +2369,7 @@
       <c r="AA14" s="10">
         <v>0.08</v>
       </c>
-      <c r="AB14" s="16">
+      <c r="AB14" s="15">
         <v>0.5</v>
       </c>
       <c r="AC14" s="10">
@@ -2328,7 +2388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:34" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>28</v>
       </c>
@@ -2377,7 +2437,7 @@
       <c r="P15" s="5">
         <v>35.92</v>
       </c>
-      <c r="Q15" s="20">
+      <c r="Q15" s="19">
         <v>3.44</v>
       </c>
       <c r="R15" s="10">
@@ -2429,7 +2489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:34" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>29</v>
       </c>
@@ -2478,7 +2538,7 @@
       <c r="P16" s="5">
         <v>14.62</v>
       </c>
-      <c r="Q16" s="20">
+      <c r="Q16" s="19">
         <v>1.73</v>
       </c>
       <c r="R16" s="10">
@@ -2564,7 +2624,7 @@
       <c r="K17" s="5">
         <v>3.78</v>
       </c>
-      <c r="L17" s="19">
+      <c r="L17" s="18">
         <v>5</v>
       </c>
       <c r="M17" s="4">
@@ -2579,7 +2639,7 @@
       <c r="P17" s="5">
         <v>0</v>
       </c>
-      <c r="Q17" s="20">
+      <c r="Q17" s="19">
         <v>17.3</v>
       </c>
       <c r="R17" s="10">
@@ -2665,13 +2725,13 @@
       <c r="K18" s="5">
         <v>4.9000000000000004</v>
       </c>
-      <c r="L18" s="19">
+      <c r="L18" s="18">
         <v>2.12</v>
       </c>
       <c r="M18" s="4">
         <v>8.14</v>
       </c>
-      <c r="N18" s="21">
+      <c r="N18" s="20">
         <v>8.3000000000000007</v>
       </c>
       <c r="O18" s="5">
@@ -2680,7 +2740,7 @@
       <c r="P18" s="5">
         <v>15.94</v>
       </c>
-      <c r="Q18" s="20">
+      <c r="Q18" s="19">
         <v>17.899999999999999</v>
       </c>
       <c r="R18" s="10">
@@ -2781,7 +2841,7 @@
       <c r="P19" s="5">
         <v>11.72</v>
       </c>
-      <c r="Q19" s="20">
+      <c r="Q19" s="19">
         <v>8.19</v>
       </c>
       <c r="R19" s="10">
@@ -2790,7 +2850,7 @@
       <c r="S19" s="10">
         <v>0</v>
       </c>
-      <c r="T19" s="16">
+      <c r="T19" s="15">
         <v>2.7</v>
       </c>
       <c r="U19" s="10">
@@ -2882,7 +2942,7 @@
       <c r="P20" s="5">
         <v>14.38</v>
       </c>
-      <c r="Q20" s="20">
+      <c r="Q20" s="19">
         <v>9.92</v>
       </c>
       <c r="R20" s="10">
@@ -2983,7 +3043,7 @@
       <c r="P21" s="5">
         <v>12.77</v>
       </c>
-      <c r="Q21" s="20">
+      <c r="Q21" s="19">
         <v>4.1399999999999997</v>
       </c>
       <c r="R21" s="10">
@@ -2995,7 +3055,7 @@
       <c r="T21" s="10">
         <v>7.83</v>
       </c>
-      <c r="U21" s="16">
+      <c r="U21" s="15">
         <v>4.3</v>
       </c>
       <c r="V21" s="10">
@@ -3007,7 +3067,7 @@
       <c r="X21" s="10">
         <v>98.49</v>
       </c>
-      <c r="Y21" s="16">
+      <c r="Y21" s="15">
         <v>4.3</v>
       </c>
       <c r="Z21" s="10">
@@ -3019,7 +3079,7 @@
       <c r="AB21" s="10">
         <v>98.49</v>
       </c>
-      <c r="AC21" s="16">
+      <c r="AC21" s="15">
         <v>4.3</v>
       </c>
       <c r="AD21" s="10">
@@ -3031,7 +3091,7 @@
       <c r="AF21" s="10">
         <v>98.49</v>
       </c>
-      <c r="AG21" s="16">
+      <c r="AG21" s="15">
         <v>4.3</v>
       </c>
     </row>
@@ -3084,7 +3144,7 @@
       <c r="P22" s="5">
         <v>20.49</v>
       </c>
-      <c r="Q22" s="20">
+      <c r="Q22" s="19">
         <v>0.61</v>
       </c>
       <c r="R22" s="10">
@@ -3185,7 +3245,7 @@
       <c r="P23" s="5">
         <v>14.51</v>
       </c>
-      <c r="Q23" s="20">
+      <c r="Q23" s="19">
         <v>3.66</v>
       </c>
       <c r="R23" s="10">
@@ -3221,7 +3281,7 @@
       <c r="AB23" s="10">
         <v>91.88</v>
       </c>
-      <c r="AC23" s="17">
+      <c r="AC23" s="16">
         <v>1.06</v>
       </c>
       <c r="AD23" s="10">
@@ -3233,7 +3293,7 @@
       <c r="AF23" s="10">
         <v>91.88</v>
       </c>
-      <c r="AG23" s="17">
+      <c r="AG23" s="16">
         <v>1.06</v>
       </c>
     </row>
@@ -3286,7 +3346,7 @@
       <c r="P24" s="5">
         <v>10.07</v>
       </c>
-      <c r="Q24" s="20">
+      <c r="Q24" s="19">
         <v>3.82</v>
       </c>
       <c r="R24" s="10">
@@ -3387,7 +3447,7 @@
       <c r="P25" s="5">
         <v>5.4</v>
       </c>
-      <c r="Q25" s="20">
+      <c r="Q25" s="19">
         <v>2.15</v>
       </c>
       <c r="R25" s="10">
@@ -3396,7 +3456,7 @@
       <c r="S25" s="10">
         <v>0</v>
       </c>
-      <c r="T25" s="16">
+      <c r="T25" s="15">
         <v>16.7</v>
       </c>
       <c r="U25" s="10">
@@ -3408,7 +3468,7 @@
       <c r="W25" s="10">
         <v>0</v>
       </c>
-      <c r="X25" s="16">
+      <c r="X25" s="15">
         <v>16.7</v>
       </c>
       <c r="Y25" s="10">
@@ -3420,7 +3480,7 @@
       <c r="AA25" s="10">
         <v>10.210000000000001</v>
       </c>
-      <c r="AB25" s="16">
+      <c r="AB25" s="15">
         <v>16.7</v>
       </c>
       <c r="AC25" s="10">
@@ -3432,10 +3492,10 @@
       <c r="AE25" s="10">
         <v>10.210000000000001</v>
       </c>
-      <c r="AF25" s="18">
+      <c r="AF25" s="17">
         <v>16.7</v>
       </c>
-      <c r="AG25" s="17">
+      <c r="AG25" s="16">
         <v>22.99</v>
       </c>
     </row>
@@ -3488,13 +3548,13 @@
       <c r="P26" s="5">
         <v>44.79</v>
       </c>
-      <c r="Q26" s="20">
+      <c r="Q26" s="19">
         <v>4.34</v>
       </c>
       <c r="R26" s="10">
         <v>0</v>
       </c>
-      <c r="S26" s="16">
+      <c r="S26" s="15">
         <v>1.5</v>
       </c>
       <c r="T26" s="10">
@@ -3589,7 +3649,7 @@
       <c r="P27" s="5">
         <v>22.49</v>
       </c>
-      <c r="Q27" s="22">
+      <c r="Q27" s="21">
         <v>11.9</v>
       </c>
       <c r="R27" s="10">
@@ -3690,7 +3750,7 @@
       <c r="P28" s="5">
         <v>7.86</v>
       </c>
-      <c r="Q28" s="20">
+      <c r="Q28" s="19">
         <v>6.26</v>
       </c>
       <c r="R28" s="10">
@@ -3717,7 +3777,7 @@
       <c r="Y28" s="10">
         <v>0</v>
       </c>
-      <c r="Z28" s="15">
+      <c r="Z28" s="14">
         <v>23</v>
       </c>
       <c r="AA28" s="10">
@@ -3729,10 +3789,10 @@
       <c r="AC28" s="10">
         <v>0</v>
       </c>
-      <c r="AD28" s="15">
+      <c r="AD28" s="14">
         <v>23</v>
       </c>
-      <c r="AE28" s="16">
+      <c r="AE28" s="15">
         <v>21.1</v>
       </c>
       <c r="AF28" s="10">
@@ -3791,7 +3851,7 @@
       <c r="P29" s="5">
         <v>0</v>
       </c>
-      <c r="Q29" s="20">
+      <c r="Q29" s="19">
         <v>6.71</v>
       </c>
       <c r="R29" s="10">
@@ -3892,7 +3952,7 @@
       <c r="P30" s="5">
         <v>0.46</v>
       </c>
-      <c r="Q30" s="20">
+      <c r="Q30" s="19">
         <v>2.67</v>
       </c>
       <c r="R30" s="10">
@@ -3993,7 +4053,7 @@
       <c r="P31" s="5">
         <v>0.51</v>
       </c>
-      <c r="Q31" s="20">
+      <c r="Q31" s="19">
         <v>0.33</v>
       </c>
       <c r="R31" s="10">
@@ -4002,7 +4062,7 @@
       <c r="S31" s="10">
         <v>6.11</v>
       </c>
-      <c r="T31" s="16">
+      <c r="T31" s="15">
         <v>44.54</v>
       </c>
       <c r="U31" s="10">
@@ -4014,7 +4074,7 @@
       <c r="W31" s="10">
         <v>25.11</v>
       </c>
-      <c r="X31" s="16">
+      <c r="X31" s="15">
         <v>44.54</v>
       </c>
       <c r="Y31" s="10">
@@ -4048,4 +4108,316 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{191690F3-C00A-624F-AD30-A957AF041456}">
+  <dimension ref="B2:K10"/>
+  <sheetViews>
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="14.6640625" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" customWidth="1"/>
+    <col min="8" max="8" width="14" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" customWidth="1"/>
+    <col min="10" max="10" width="14" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:11" ht="27" x14ac:dyDescent="0.2">
+      <c r="B2" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="24" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B3" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="30">
+        <v>106.8</v>
+      </c>
+      <c r="E3" s="27">
+        <v>13.3</v>
+      </c>
+      <c r="F3" s="26">
+        <v>3.3</v>
+      </c>
+      <c r="G3" s="26">
+        <v>12.4</v>
+      </c>
+      <c r="H3" s="32">
+        <v>28.5</v>
+      </c>
+      <c r="I3" s="27">
+        <v>53.3</v>
+      </c>
+      <c r="J3" s="27">
+        <v>4.8</v>
+      </c>
+      <c r="K3" s="27">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B4" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="30">
+        <v>2.1</v>
+      </c>
+      <c r="E4" s="27">
+        <v>7.5</v>
+      </c>
+      <c r="F4" s="26">
+        <v>0.8</v>
+      </c>
+      <c r="G4" s="26">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H4" s="32">
+        <v>20.8</v>
+      </c>
+      <c r="I4" s="27">
+        <v>39.700000000000003</v>
+      </c>
+      <c r="J4" s="27">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="K4" s="27">
+        <v>14.3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B5" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="30">
+        <v>0.4</v>
+      </c>
+      <c r="E5" s="27">
+        <v>6.3</v>
+      </c>
+      <c r="F5" s="26">
+        <v>20.6</v>
+      </c>
+      <c r="G5" s="26">
+        <v>0</v>
+      </c>
+      <c r="H5" s="32">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="I5" s="27">
+        <v>55.3</v>
+      </c>
+      <c r="J5" s="27">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="K5" s="27">
+        <v>12.7</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B6" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="33">
+        <v>1.5</v>
+      </c>
+      <c r="E6" s="34">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="F6" s="35">
+        <v>2.1</v>
+      </c>
+      <c r="G6" s="26">
+        <v>8.1</v>
+      </c>
+      <c r="H6" s="36">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="I6" s="27">
+        <v>39.700000000000003</v>
+      </c>
+      <c r="J6" s="27">
+        <v>15.9</v>
+      </c>
+      <c r="K6" s="34">
+        <v>17.899999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B7" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="30">
+        <v>1.2</v>
+      </c>
+      <c r="E7" s="27">
+        <v>13.1</v>
+      </c>
+      <c r="F7" s="35">
+        <v>10</v>
+      </c>
+      <c r="G7" s="26">
+        <v>0</v>
+      </c>
+      <c r="H7" s="36">
+        <v>8</v>
+      </c>
+      <c r="I7" s="27">
+        <v>64.400000000000006</v>
+      </c>
+      <c r="J7" s="27">
+        <v>14.4</v>
+      </c>
+      <c r="K7" s="27">
+        <v>9.9</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B8" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="30">
+        <v>1.7</v>
+      </c>
+      <c r="E8" s="27">
+        <v>13.1</v>
+      </c>
+      <c r="F8" s="26">
+        <v>0.6</v>
+      </c>
+      <c r="G8" s="26">
+        <v>1.2</v>
+      </c>
+      <c r="H8" s="32">
+        <v>66.8</v>
+      </c>
+      <c r="I8" s="27">
+        <v>20.7</v>
+      </c>
+      <c r="J8" s="27">
+        <v>0</v>
+      </c>
+      <c r="K8" s="27">
+        <v>6.7</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B9" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="30">
+        <v>11.6</v>
+      </c>
+      <c r="E9" s="27">
+        <v>14.3</v>
+      </c>
+      <c r="F9" s="26">
+        <v>1.7</v>
+      </c>
+      <c r="G9" s="35">
+        <v>3.9</v>
+      </c>
+      <c r="H9" s="36">
+        <v>68.8</v>
+      </c>
+      <c r="I9" s="27">
+        <v>22.8</v>
+      </c>
+      <c r="J9" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="K9" s="27">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B10" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="33">
+        <v>14.2</v>
+      </c>
+      <c r="E10" s="27">
+        <v>10.7</v>
+      </c>
+      <c r="F10" s="26">
+        <v>5.3</v>
+      </c>
+      <c r="G10" s="26">
+        <v>4.2</v>
+      </c>
+      <c r="H10" s="32">
+        <v>78.3</v>
+      </c>
+      <c r="I10" s="27">
+        <v>15.2</v>
+      </c>
+      <c r="J10" s="27">
+        <v>0.51</v>
+      </c>
+      <c r="K10" s="27">
+        <v>0.3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
upd - checked the math on instantaneous flux and re-checked that the daily discharge values were correctly pulled from the XX_dailyQ.RDS files.
</commit_message>
<xml_diff>
--- a/Watershed_table_v1.xlsx
+++ b/Watershed_table_v1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/MW/2020 Trent University/R/Thesis Data/MSc_data_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59F7C266-3A6C-494F-BD3B-76605599052A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{732DF53C-B433-4F48-9EA2-380D2A267CFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9600" yWindow="2300" windowWidth="28800" windowHeight="17500" xr2:uid="{3AD1715B-176F-3140-B9AE-F64F14EE2DEE}"/>
+    <workbookView xWindow="9180" yWindow="680" windowWidth="29080" windowHeight="8440" xr2:uid="{3AD1715B-176F-3140-B9AE-F64F14EE2DEE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -320,45 +320,6 @@
     <t>Poor</t>
   </si>
   <si>
-    <t>5-year abiotic disturbance (%)</t>
-  </si>
-  <si>
-    <t>10-year wildfire disturbance (%)</t>
-  </si>
-  <si>
-    <t>10-year harvest disturbance (%)</t>
-  </si>
-  <si>
-    <t>10-year insect disturbance (%)</t>
-  </si>
-  <si>
-    <t>10-year abiotic disturbance (%)</t>
-  </si>
-  <si>
-    <t>20-year wildfire disturbance (%)</t>
-  </si>
-  <si>
-    <t>20-year harvest disturbance (%)</t>
-  </si>
-  <si>
-    <t>20-year insect disturbance (%)</t>
-  </si>
-  <si>
-    <t>20-year abiotic disturbance (%)</t>
-  </si>
-  <si>
-    <t>15-year wildfire disturbance (%)</t>
-  </si>
-  <si>
-    <t>15-year harvest disturbance (%)</t>
-  </si>
-  <si>
-    <t>15-year insect disturbance (%)</t>
-  </si>
-  <si>
-    <t>15-year abiotic disturbance (%)</t>
-  </si>
-  <si>
     <t>5-year Wildfire Disturbance (%)</t>
   </si>
   <si>
@@ -369,6 +330,45 @@
   </si>
   <si>
     <t>Sparse Forest (%)</t>
+  </si>
+  <si>
+    <t>5-year Abiotic Disturbance (%)</t>
+  </si>
+  <si>
+    <t>10-year Wildfire Disturbance (%)</t>
+  </si>
+  <si>
+    <t>10-year Harvest Disturbance (%)</t>
+  </si>
+  <si>
+    <t>10-year Insect Disturbance (%)</t>
+  </si>
+  <si>
+    <t>10-year Abiotic Disturbance (%)</t>
+  </si>
+  <si>
+    <t>15-year Wildfire Disturbance (%)</t>
+  </si>
+  <si>
+    <t>15-year Harvest Disturbance (%)</t>
+  </si>
+  <si>
+    <t>15-year Insect Disturbance (%)</t>
+  </si>
+  <si>
+    <t>15-year Abiotic Disturbance (%)</t>
+  </si>
+  <si>
+    <t>20-year Wildfire Disturbance (%)</t>
+  </si>
+  <si>
+    <t>20-year Harvest Disturbance (%)</t>
+  </si>
+  <si>
+    <t>20-year Insect Disturbance (%)</t>
+  </si>
+  <si>
+    <t>20-year Abiotic Disturbance (%)</t>
   </si>
 </sst>
 </file>
@@ -547,7 +547,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -585,10 +585,6 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -643,6 +639,13 @@
     <xf numFmtId="164" fontId="4" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -960,10 +963,10 @@
   <dimension ref="A1:AG31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="174" zoomScaleNormal="162" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="I7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A18" sqref="A18:XFD18"/>
+      <selection pane="bottomRight" activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1024,31 +1027,31 @@
         <v>11</v>
       </c>
       <c r="Q1" s="9" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="R1" s="9" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="S1" s="9" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="T1" s="9" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="U1" s="9" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="V1" s="12" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="W1" s="12" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="X1" s="12" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="Y1" s="12" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="Z1" s="12" t="s">
         <v>95</v>
@@ -1063,16 +1066,16 @@
         <v>98</v>
       </c>
       <c r="AD1" s="12" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="AE1" s="12" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="AF1" s="12" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="AG1" s="12" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1101,19 +1104,19 @@
         <v>-84.049700000000001</v>
       </c>
       <c r="I2" s="4">
-        <v>15.59</v>
+        <v>15.6</v>
       </c>
       <c r="J2" s="4">
-        <v>465.85</v>
+        <v>465.9</v>
       </c>
       <c r="K2" s="5">
-        <v>7.75</v>
-      </c>
-      <c r="L2" s="4">
-        <v>3.03</v>
+        <v>7.8</v>
+      </c>
+      <c r="L2" s="20">
+        <v>0.5</v>
       </c>
       <c r="M2" s="4">
-        <v>4.47</v>
+        <v>4.5</v>
       </c>
       <c r="N2" s="5">
         <v>7.57</v>
@@ -1124,7 +1127,7 @@
       <c r="P2" s="5">
         <v>12.43</v>
       </c>
-      <c r="Q2" s="19">
+      <c r="Q2" s="17">
         <v>2.61</v>
       </c>
       <c r="R2" s="10">
@@ -1155,7 +1158,7 @@
         <v>0</v>
       </c>
       <c r="AA2" s="10">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="AB2" s="10">
         <v>0</v>
@@ -1167,7 +1170,7 @@
         <v>0</v>
       </c>
       <c r="AE2" s="10">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="AF2" s="10">
         <v>100</v>
@@ -1202,19 +1205,19 @@
         <v>-84.764600000000002</v>
       </c>
       <c r="I3" s="4">
-        <v>30.57</v>
+        <v>30.6</v>
       </c>
       <c r="J3" s="4">
-        <v>339.27</v>
+        <v>339.3</v>
       </c>
       <c r="K3" s="5">
-        <v>12.23</v>
+        <v>12.2</v>
       </c>
       <c r="L3" s="4">
-        <v>0.94</v>
-      </c>
-      <c r="M3" s="4">
-        <v>27.02</v>
+        <v>0.9</v>
+      </c>
+      <c r="M3" s="20">
+        <v>27</v>
       </c>
       <c r="N3" s="5">
         <v>17.72</v>
@@ -1225,7 +1228,7 @@
       <c r="P3" s="5">
         <v>3.61</v>
       </c>
-      <c r="Q3" s="19">
+      <c r="Q3" s="17">
         <v>0.97</v>
       </c>
       <c r="R3" s="10">
@@ -1303,19 +1306,19 @@
         <v>-84.648399999999995</v>
       </c>
       <c r="I4" s="4">
-        <v>12.82</v>
+        <v>12.8</v>
       </c>
       <c r="J4" s="4">
-        <v>365.39</v>
+        <v>365.4</v>
       </c>
       <c r="K4" s="5">
-        <v>8.56</v>
+        <v>8.6</v>
       </c>
       <c r="L4" s="4">
         <v>6.2</v>
       </c>
       <c r="M4" s="4">
-        <v>12.73</v>
+        <v>12.7</v>
       </c>
       <c r="N4" s="5">
         <v>23.18</v>
@@ -1326,7 +1329,7 @@
       <c r="P4" s="5">
         <v>3.95</v>
       </c>
-      <c r="Q4" s="19">
+      <c r="Q4" s="17">
         <v>1.46</v>
       </c>
       <c r="R4" s="10">
@@ -1404,19 +1407,19 @@
         <v>-84.390900000000002</v>
       </c>
       <c r="I5" s="4">
-        <v>106.77</v>
+        <v>106.8</v>
       </c>
       <c r="J5" s="4">
-        <v>440.28</v>
+        <v>440.3</v>
       </c>
       <c r="K5" s="5">
-        <v>13.27</v>
+        <v>13.3</v>
       </c>
       <c r="L5" s="4">
-        <v>3.26</v>
+        <v>3.3</v>
       </c>
       <c r="M5" s="4">
-        <v>12.36</v>
+        <v>12.4</v>
       </c>
       <c r="N5" s="5">
         <v>28.52</v>
@@ -1427,7 +1430,7 @@
       <c r="P5" s="5">
         <v>4.8099999999999996</v>
       </c>
-      <c r="Q5" s="19">
+      <c r="Q5" s="17">
         <v>3.44</v>
       </c>
       <c r="R5" s="10">
@@ -1505,19 +1508,19 @@
         <v>-84.367199999999997</v>
       </c>
       <c r="I6" s="4">
-        <v>39.32</v>
-      </c>
-      <c r="J6" s="4">
-        <v>395</v>
+        <v>39.299999999999997</v>
+      </c>
+      <c r="J6" s="20">
+        <v>394.9</v>
       </c>
       <c r="K6" s="5">
-        <v>12.24</v>
-      </c>
-      <c r="L6" s="4">
-        <v>1.01</v>
+        <v>12.2</v>
+      </c>
+      <c r="L6" s="20">
+        <v>0.4</v>
       </c>
       <c r="M6" s="4">
-        <v>3.71</v>
+        <v>3.7</v>
       </c>
       <c r="N6" s="5">
         <v>18.52</v>
@@ -1528,7 +1531,7 @@
       <c r="P6" s="5">
         <v>5.53</v>
       </c>
-      <c r="Q6" s="19">
+      <c r="Q6" s="17">
         <v>1.48</v>
       </c>
       <c r="R6" s="10">
@@ -1606,19 +1609,19 @@
         <v>-84.348500000000001</v>
       </c>
       <c r="I7" s="4">
-        <v>1.77</v>
+        <v>1.8</v>
       </c>
       <c r="J7" s="4">
-        <v>385.33</v>
+        <v>385.3</v>
       </c>
       <c r="K7" s="5">
-        <v>6.24</v>
+        <v>6.2</v>
       </c>
       <c r="L7" s="4">
         <v>7.8</v>
       </c>
       <c r="M7" s="4">
-        <v>0.74</v>
+        <v>0.7</v>
       </c>
       <c r="N7" s="5">
         <v>15.18</v>
@@ -1629,7 +1632,7 @@
       <c r="P7" s="5">
         <v>5.1100000000000003</v>
       </c>
-      <c r="Q7" s="19">
+      <c r="Q7" s="17">
         <v>3.87</v>
       </c>
       <c r="R7" s="10">
@@ -1707,19 +1710,19 @@
         <v>-84.174700000000001</v>
       </c>
       <c r="I8" s="4">
-        <v>2.08</v>
-      </c>
-      <c r="J8" s="4">
+        <v>2.1</v>
+      </c>
+      <c r="J8" s="20">
         <v>431</v>
       </c>
       <c r="K8" s="5">
-        <v>7.45</v>
+        <v>7.5</v>
       </c>
       <c r="L8" s="4">
-        <v>0.82</v>
+        <v>0</v>
       </c>
       <c r="M8" s="4">
-        <v>1.1299999999999999</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="N8" s="5">
         <v>20.83</v>
@@ -1730,14 +1733,14 @@
       <c r="P8" s="5">
         <v>16.91</v>
       </c>
-      <c r="Q8" s="19">
+      <c r="Q8" s="17">
         <v>14.34</v>
       </c>
       <c r="R8" s="10">
         <v>0</v>
       </c>
       <c r="S8" s="10">
-        <v>32.33</v>
+        <v>32.299999999999997</v>
       </c>
       <c r="T8" s="10">
         <v>0</v>
@@ -1746,10 +1749,10 @@
         <v>0</v>
       </c>
       <c r="V8" s="10">
-        <v>25.27</v>
+        <v>25.3</v>
       </c>
       <c r="W8" s="10">
-        <v>32.33</v>
+        <v>32.299999999999997</v>
       </c>
       <c r="X8" s="10">
         <v>0</v>
@@ -1758,10 +1761,10 @@
         <v>0</v>
       </c>
       <c r="Z8" s="10">
-        <v>25.27</v>
+        <v>25.3</v>
       </c>
       <c r="AA8" s="10">
-        <v>32.33</v>
+        <v>32.299999999999997</v>
       </c>
       <c r="AB8" s="10">
         <v>0</v>
@@ -1770,10 +1773,10 @@
         <v>0</v>
       </c>
       <c r="AD8" s="13">
-        <v>25.27</v>
+        <v>25.3</v>
       </c>
       <c r="AE8" s="10">
-        <v>32.33</v>
+        <v>32.299999999999997</v>
       </c>
       <c r="AF8" s="10">
         <v>100</v>
@@ -1808,21 +1811,21 @@
         <v>-84.107900000000001</v>
       </c>
       <c r="I9" s="4">
-        <v>4.55</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="J9" s="4">
-        <v>454.09</v>
+        <v>454.1</v>
       </c>
       <c r="K9" s="5">
-        <v>7.21</v>
-      </c>
-      <c r="L9" s="22">
+        <v>7.2</v>
+      </c>
+      <c r="L9" s="20">
         <v>11.6</v>
       </c>
-      <c r="M9" s="18">
+      <c r="M9" s="20">
         <v>4.9000000000000004</v>
       </c>
-      <c r="N9" s="20">
+      <c r="N9" s="18">
         <v>18.5</v>
       </c>
       <c r="O9" s="5">
@@ -1831,7 +1834,7 @@
       <c r="P9" s="5">
         <v>7.61</v>
       </c>
-      <c r="Q9" s="19">
+      <c r="Q9" s="17">
         <v>15.21</v>
       </c>
       <c r="R9" s="10">
@@ -1909,16 +1912,16 @@
         <v>-84.180499999999995</v>
       </c>
       <c r="I10" s="4">
-        <v>0.43</v>
+        <v>0.5</v>
       </c>
       <c r="J10" s="4">
-        <v>427.45</v>
+        <v>427.5</v>
       </c>
       <c r="K10" s="5">
-        <v>6.29</v>
+        <v>6.3</v>
       </c>
       <c r="L10" s="4">
-        <v>20.6</v>
+        <v>0.1</v>
       </c>
       <c r="M10" s="4">
         <v>0</v>
@@ -1932,14 +1935,14 @@
       <c r="P10" s="5">
         <v>19.350000000000001</v>
       </c>
-      <c r="Q10" s="19">
+      <c r="Q10" s="17">
         <v>12.69</v>
       </c>
       <c r="R10" s="10">
         <v>0</v>
       </c>
       <c r="S10" s="10">
-        <v>52.48</v>
+        <v>52.5</v>
       </c>
       <c r="T10" s="10">
         <v>0</v>
@@ -1951,7 +1954,7 @@
         <v>0</v>
       </c>
       <c r="W10" s="10">
-        <v>52.48</v>
+        <v>52.5</v>
       </c>
       <c r="X10" s="10">
         <v>0</v>
@@ -1963,7 +1966,7 @@
         <v>0</v>
       </c>
       <c r="AA10" s="10">
-        <v>52.48</v>
+        <v>52.5</v>
       </c>
       <c r="AB10" s="10">
         <v>0</v>
@@ -1975,7 +1978,7 @@
         <v>0</v>
       </c>
       <c r="AE10" s="10">
-        <v>52.48</v>
+        <v>52.5</v>
       </c>
       <c r="AF10" s="10">
         <v>0</v>
@@ -2010,19 +2013,19 @@
         <v>-83.904700000000005</v>
       </c>
       <c r="I11" s="4">
-        <v>1.22</v>
+        <v>1.2</v>
       </c>
       <c r="J11" s="4">
-        <v>449.34</v>
+        <v>449.3</v>
       </c>
       <c r="K11" s="5">
-        <v>4.5199999999999996</v>
+        <v>4.5</v>
       </c>
       <c r="L11" s="4">
-        <v>11.07</v>
-      </c>
-      <c r="M11" s="4">
-        <v>4.97</v>
+        <v>0.1</v>
+      </c>
+      <c r="M11" s="20">
+        <v>5</v>
       </c>
       <c r="N11" s="5">
         <v>2.44</v>
@@ -2033,7 +2036,7 @@
       <c r="P11" s="5">
         <v>4.21</v>
       </c>
-      <c r="Q11" s="19">
+      <c r="Q11" s="17">
         <v>17.64</v>
       </c>
       <c r="R11" s="10">
@@ -2114,16 +2117,16 @@
         <v>69.3</v>
       </c>
       <c r="J12" s="4">
-        <v>459.51</v>
+        <v>459.5</v>
       </c>
       <c r="K12" s="5">
         <v>4.5</v>
       </c>
       <c r="L12" s="4">
-        <v>2.64</v>
+        <v>1.8</v>
       </c>
       <c r="M12" s="4">
-        <v>5.32</v>
+        <v>5.3</v>
       </c>
       <c r="N12" s="5">
         <v>11.62</v>
@@ -2134,7 +2137,7 @@
       <c r="P12" s="5">
         <v>18.12</v>
       </c>
-      <c r="Q12" s="19">
+      <c r="Q12" s="17">
         <v>3.91</v>
       </c>
       <c r="R12" s="10">
@@ -2165,7 +2168,7 @@
         <v>0</v>
       </c>
       <c r="AA12" s="10">
-        <v>0.42</v>
+        <v>0.4</v>
       </c>
       <c r="AB12" s="10">
         <v>0</v>
@@ -2177,7 +2180,7 @@
         <v>0</v>
       </c>
       <c r="AE12" s="10">
-        <v>1.88</v>
+        <v>1.9</v>
       </c>
       <c r="AF12" s="10">
         <v>100</v>
@@ -2212,19 +2215,19 @@
         <v>-83.831599999999995</v>
       </c>
       <c r="I13" s="4">
-        <v>20.46</v>
+        <v>20.5</v>
       </c>
       <c r="J13" s="4">
-        <v>454.71</v>
+        <v>454.7</v>
       </c>
       <c r="K13" s="5">
-        <v>3.74</v>
+        <v>3.7</v>
       </c>
       <c r="L13" s="4">
-        <v>5.88</v>
+        <v>1.2</v>
       </c>
       <c r="M13" s="4">
-        <v>32.729999999999997</v>
+        <v>32.700000000000003</v>
       </c>
       <c r="N13" s="5">
         <v>3.26</v>
@@ -2235,7 +2238,7 @@
       <c r="P13" s="5">
         <v>22.66</v>
       </c>
-      <c r="Q13" s="19">
+      <c r="Q13" s="17">
         <v>4.62</v>
       </c>
       <c r="R13" s="10">
@@ -2278,7 +2281,7 @@
         <v>0</v>
       </c>
       <c r="AE13" s="10">
-        <v>1.31</v>
+        <v>1.3</v>
       </c>
       <c r="AF13" s="10">
         <v>100</v>
@@ -2313,16 +2316,16 @@
         <v>-83.770099999999999</v>
       </c>
       <c r="I14" s="4">
-        <v>13.07</v>
+        <v>13.1</v>
       </c>
       <c r="J14" s="4">
-        <v>464.84</v>
+        <v>464.8</v>
       </c>
       <c r="K14" s="5">
-        <v>5.48</v>
+        <v>5.5</v>
       </c>
       <c r="L14" s="4">
-        <v>4.3099999999999996</v>
+        <v>0.6</v>
       </c>
       <c r="M14" s="4">
         <v>20.8</v>
@@ -2336,14 +2339,14 @@
       <c r="P14" s="5">
         <v>8.15</v>
       </c>
-      <c r="Q14" s="19">
+      <c r="Q14" s="17">
         <v>4.7699999999999996</v>
       </c>
       <c r="R14" s="10">
         <v>0</v>
       </c>
       <c r="S14" s="10">
-        <v>0.08</v>
+        <v>0.1</v>
       </c>
       <c r="T14" s="10">
         <v>0</v>
@@ -2355,9 +2358,9 @@
         <v>0</v>
       </c>
       <c r="W14" s="10">
-        <v>0.08</v>
-      </c>
-      <c r="X14" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="X14" s="14">
         <v>0.5</v>
       </c>
       <c r="Y14" s="10">
@@ -2367,9 +2370,9 @@
         <v>0</v>
       </c>
       <c r="AA14" s="10">
-        <v>0.08</v>
-      </c>
-      <c r="AB14" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="AB14" s="14">
         <v>0.5</v>
       </c>
       <c r="AC14" s="10">
@@ -2379,7 +2382,7 @@
         <v>0</v>
       </c>
       <c r="AE14" s="10">
-        <v>1.54</v>
+        <v>1.5</v>
       </c>
       <c r="AF14" s="10">
         <v>100</v>
@@ -2414,19 +2417,19 @@
         <v>-83.634100000000004</v>
       </c>
       <c r="I15" s="4">
-        <v>5.17</v>
+        <v>5.2</v>
       </c>
       <c r="J15" s="4">
-        <v>473.23</v>
+        <v>473.2</v>
       </c>
       <c r="K15" s="5">
-        <v>4.58</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="L15" s="4">
         <v>7.6</v>
       </c>
       <c r="M15" s="4">
-        <v>0.31</v>
+        <v>0.3</v>
       </c>
       <c r="N15" s="5">
         <v>18.12</v>
@@ -2437,17 +2440,17 @@
       <c r="P15" s="5">
         <v>35.92</v>
       </c>
-      <c r="Q15" s="19">
+      <c r="Q15" s="17">
         <v>3.44</v>
       </c>
       <c r="R15" s="10">
         <v>0</v>
       </c>
       <c r="S15" s="10">
-        <v>38.28</v>
+        <v>38.299999999999997</v>
       </c>
       <c r="T15" s="10">
-        <v>1.1599999999999999</v>
+        <v>1.2</v>
       </c>
       <c r="U15" s="10">
         <v>0</v>
@@ -2456,10 +2459,10 @@
         <v>0</v>
       </c>
       <c r="W15" s="10">
-        <v>38.28</v>
+        <v>38.299999999999997</v>
       </c>
       <c r="X15" s="10">
-        <v>94.27</v>
+        <v>94.3</v>
       </c>
       <c r="Y15" s="10">
         <v>0</v>
@@ -2468,10 +2471,10 @@
         <v>0</v>
       </c>
       <c r="AA15" s="10">
-        <v>38.28</v>
+        <v>38.299999999999997</v>
       </c>
       <c r="AB15" s="10">
-        <v>94.27</v>
+        <v>94.3</v>
       </c>
       <c r="AC15" s="10">
         <v>0</v>
@@ -2480,10 +2483,10 @@
         <v>0</v>
       </c>
       <c r="AE15" s="10">
-        <v>38.28</v>
+        <v>38.299999999999997</v>
       </c>
       <c r="AF15" s="10">
-        <v>98.47</v>
+        <v>98.5</v>
       </c>
       <c r="AG15" s="10">
         <v>0</v>
@@ -2518,16 +2521,16 @@
         <v>1.8</v>
       </c>
       <c r="J16" s="4">
-        <v>483.19</v>
+        <v>483.2</v>
       </c>
       <c r="K16" s="5">
-        <v>7.17</v>
+        <v>7.2</v>
       </c>
       <c r="L16" s="4">
-        <v>3.23</v>
+        <v>3.2</v>
       </c>
       <c r="M16" s="4">
-        <v>2.2400000000000002</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="N16" s="5">
         <v>44.57</v>
@@ -2538,14 +2541,14 @@
       <c r="P16" s="5">
         <v>14.62</v>
       </c>
-      <c r="Q16" s="19">
+      <c r="Q16" s="17">
         <v>1.73</v>
       </c>
       <c r="R16" s="10">
         <v>0</v>
       </c>
       <c r="S16" s="10">
-        <v>21.38</v>
+        <v>21.4</v>
       </c>
       <c r="T16" s="10">
         <v>0</v>
@@ -2557,10 +2560,10 @@
         <v>0</v>
       </c>
       <c r="W16" s="10">
-        <v>21.38</v>
+        <v>21.4</v>
       </c>
       <c r="X16" s="10">
-        <v>95.33</v>
+        <v>95.3</v>
       </c>
       <c r="Y16" s="10">
         <v>0</v>
@@ -2569,10 +2572,10 @@
         <v>0</v>
       </c>
       <c r="AA16" s="10">
-        <v>21.38</v>
+        <v>21.4</v>
       </c>
       <c r="AB16" s="10">
-        <v>95.33</v>
+        <v>95.3</v>
       </c>
       <c r="AC16" s="10">
         <v>0</v>
@@ -2581,10 +2584,10 @@
         <v>0</v>
       </c>
       <c r="AE16" s="10">
-        <v>21.38</v>
+        <v>21.4</v>
       </c>
       <c r="AF16" s="10">
-        <v>98.31</v>
+        <v>98.3</v>
       </c>
       <c r="AG16" s="10">
         <v>0</v>
@@ -2616,15 +2619,15 @@
         <v>-83.452500000000001</v>
       </c>
       <c r="I17" s="4">
-        <v>0.16900000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="J17" s="4">
-        <v>454.77</v>
+        <v>454.8</v>
       </c>
       <c r="K17" s="5">
-        <v>3.78</v>
-      </c>
-      <c r="L17" s="18">
+        <v>3.8</v>
+      </c>
+      <c r="L17" s="20">
         <v>5</v>
       </c>
       <c r="M17" s="4">
@@ -2639,7 +2642,7 @@
       <c r="P17" s="5">
         <v>0</v>
       </c>
-      <c r="Q17" s="19">
+      <c r="Q17" s="17">
         <v>17.3</v>
       </c>
       <c r="R17" s="10">
@@ -2720,18 +2723,18 @@
         <v>1.5</v>
       </c>
       <c r="J18" s="4">
-        <v>457.61</v>
+        <v>457.6</v>
       </c>
       <c r="K18" s="5">
         <v>4.9000000000000004</v>
       </c>
-      <c r="L18" s="18">
-        <v>2.12</v>
+      <c r="L18" s="36">
+        <v>0</v>
       </c>
       <c r="M18" s="4">
-        <v>8.14</v>
-      </c>
-      <c r="N18" s="20">
+        <v>8.1</v>
+      </c>
+      <c r="N18" s="18">
         <v>8.3000000000000007</v>
       </c>
       <c r="O18" s="5">
@@ -2740,7 +2743,7 @@
       <c r="P18" s="5">
         <v>15.94</v>
       </c>
-      <c r="Q18" s="19">
+      <c r="Q18" s="17">
         <v>17.899999999999999</v>
       </c>
       <c r="R18" s="10">
@@ -2818,19 +2821,19 @@
         <v>-83.142300000000006</v>
       </c>
       <c r="I19" s="4">
-        <v>46.02</v>
+        <v>46</v>
       </c>
       <c r="J19" s="4">
-        <v>477.52</v>
+        <v>477.5</v>
       </c>
       <c r="K19" s="5">
-        <v>12.14</v>
+        <v>12.1</v>
       </c>
       <c r="L19" s="4">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="M19" s="4">
-        <v>9.35</v>
+        <v>9.4</v>
       </c>
       <c r="N19" s="5">
         <v>18.63</v>
@@ -2841,7 +2844,7 @@
       <c r="P19" s="5">
         <v>11.72</v>
       </c>
-      <c r="Q19" s="19">
+      <c r="Q19" s="17">
         <v>8.19</v>
       </c>
       <c r="R19" s="10">
@@ -2850,7 +2853,7 @@
       <c r="S19" s="10">
         <v>0</v>
       </c>
-      <c r="T19" s="15">
+      <c r="T19" s="14">
         <v>2.7</v>
       </c>
       <c r="U19" s="10">
@@ -2863,7 +2866,7 @@
         <v>0</v>
       </c>
       <c r="X19" s="10">
-        <v>30.75</v>
+        <v>30.8</v>
       </c>
       <c r="Y19" s="10">
         <v>0</v>
@@ -2875,7 +2878,7 @@
         <v>0</v>
       </c>
       <c r="AB19" s="10">
-        <v>30.76</v>
+        <v>30.8</v>
       </c>
       <c r="AC19" s="10">
         <v>0</v>
@@ -2887,7 +2890,7 @@
         <v>0</v>
       </c>
       <c r="AF19" s="10">
-        <v>30.76</v>
+        <v>30.8</v>
       </c>
       <c r="AG19" s="10">
         <v>0</v>
@@ -2919,16 +2922,16 @@
         <v>-83.154200000000003</v>
       </c>
       <c r="I20" s="4">
-        <v>1.23</v>
+        <v>1.2</v>
       </c>
       <c r="J20" s="4">
-        <v>469.68</v>
+        <v>469.7</v>
       </c>
       <c r="K20" s="5">
-        <v>13.05</v>
-      </c>
-      <c r="L20" s="4">
-        <v>9.99</v>
+        <v>13.1</v>
+      </c>
+      <c r="L20" s="20">
+        <v>10</v>
       </c>
       <c r="M20" s="4">
         <v>0</v>
@@ -2942,7 +2945,7 @@
       <c r="P20" s="5">
         <v>14.38</v>
       </c>
-      <c r="Q20" s="19">
+      <c r="Q20" s="17">
         <v>9.92</v>
       </c>
       <c r="R20" s="10">
@@ -2964,7 +2967,7 @@
         <v>0</v>
       </c>
       <c r="X20" s="10">
-        <v>38.619999999999997</v>
+        <v>38.6</v>
       </c>
       <c r="Y20" s="10">
         <v>0</v>
@@ -2976,7 +2979,7 @@
         <v>0</v>
       </c>
       <c r="AB20" s="10">
-        <v>38.619999999999997</v>
+        <v>38.6</v>
       </c>
       <c r="AC20" s="10">
         <v>0</v>
@@ -2988,7 +2991,7 @@
         <v>0</v>
       </c>
       <c r="AF20" s="10">
-        <v>38.619999999999997</v>
+        <v>38.6</v>
       </c>
       <c r="AG20" s="10">
         <v>0</v>
@@ -3020,19 +3023,19 @@
         <v>-83.203599999999994</v>
       </c>
       <c r="I21" s="4">
-        <v>19.55</v>
+        <v>19.600000000000001</v>
       </c>
       <c r="J21" s="4">
-        <v>514.07000000000005</v>
+        <v>514.1</v>
       </c>
       <c r="K21" s="5">
-        <v>9.8800000000000008</v>
+        <v>9.9</v>
       </c>
       <c r="L21" s="4">
-        <v>3.51</v>
+        <v>0.7</v>
       </c>
       <c r="M21" s="4">
-        <v>1.89</v>
+        <v>1.9</v>
       </c>
       <c r="N21" s="5">
         <v>37.369999999999997</v>
@@ -3043,55 +3046,55 @@
       <c r="P21" s="5">
         <v>12.77</v>
       </c>
-      <c r="Q21" s="19">
+      <c r="Q21" s="17">
         <v>4.1399999999999997</v>
       </c>
       <c r="R21" s="10">
         <v>0</v>
       </c>
       <c r="S21" s="10">
-        <v>16.05</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="T21" s="10">
-        <v>7.83</v>
-      </c>
-      <c r="U21" s="15">
+        <v>7.8</v>
+      </c>
+      <c r="U21" s="14">
         <v>4.3</v>
       </c>
       <c r="V21" s="10">
         <v>0</v>
       </c>
       <c r="W21" s="10">
-        <v>16.05</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="X21" s="10">
-        <v>98.49</v>
-      </c>
-      <c r="Y21" s="15">
+        <v>98.5</v>
+      </c>
+      <c r="Y21" s="14">
         <v>4.3</v>
       </c>
       <c r="Z21" s="10">
         <v>0</v>
       </c>
       <c r="AA21" s="10">
-        <v>16.05</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="AB21" s="10">
-        <v>98.49</v>
-      </c>
-      <c r="AC21" s="15">
+        <v>98.5</v>
+      </c>
+      <c r="AC21" s="14">
         <v>4.3</v>
       </c>
       <c r="AD21" s="10">
         <v>0</v>
       </c>
       <c r="AE21" s="10">
-        <v>16.05</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="AF21" s="10">
-        <v>98.49</v>
-      </c>
-      <c r="AG21" s="15">
+        <v>98.5</v>
+      </c>
+      <c r="AG21" s="14">
         <v>4.3</v>
       </c>
     </row>
@@ -3121,19 +3124,19 @@
         <v>-83.209900000000005</v>
       </c>
       <c r="I22" s="4">
-        <v>2.6720000000000002</v>
+        <v>2.7</v>
       </c>
       <c r="J22" s="4">
-        <v>459.47</v>
+        <v>459.5</v>
       </c>
       <c r="K22" s="5">
-        <v>3.64</v>
+        <v>3.6</v>
       </c>
       <c r="L22" s="4">
-        <v>9.1199999999999992</v>
-      </c>
-      <c r="M22" s="4">
-        <v>5.03</v>
+        <v>0.2</v>
+      </c>
+      <c r="M22" s="20">
+        <v>5</v>
       </c>
       <c r="N22" s="5">
         <v>1.04</v>
@@ -3144,7 +3147,7 @@
       <c r="P22" s="5">
         <v>20.49</v>
       </c>
-      <c r="Q22" s="19">
+      <c r="Q22" s="17">
         <v>0.61</v>
       </c>
       <c r="R22" s="10">
@@ -3153,8 +3156,8 @@
       <c r="S22" s="10">
         <v>0</v>
       </c>
-      <c r="T22" s="10">
-        <v>17.989999999999998</v>
+      <c r="T22" s="14">
+        <v>18</v>
       </c>
       <c r="U22" s="10">
         <v>0</v>
@@ -3187,7 +3190,7 @@
         <v>0</v>
       </c>
       <c r="AE22" s="10">
-        <v>24.41</v>
+        <v>24.4</v>
       </c>
       <c r="AF22" s="10">
         <v>100</v>
@@ -3221,20 +3224,20 @@
       <c r="H23" s="4">
         <v>-83.200699999999998</v>
       </c>
-      <c r="I23" s="4">
-        <v>36.020000000000003</v>
+      <c r="I23" s="20">
+        <v>36</v>
       </c>
       <c r="J23" s="4">
-        <v>482.33</v>
-      </c>
-      <c r="K23" s="5">
-        <v>5.97</v>
+        <v>482.3</v>
+      </c>
+      <c r="K23" s="35">
+        <v>6</v>
       </c>
       <c r="L23" s="4">
-        <v>3.54</v>
+        <v>1.3</v>
       </c>
       <c r="M23" s="4">
-        <v>4.7300000000000004</v>
+        <v>4.7</v>
       </c>
       <c r="N23" s="5">
         <v>28.98</v>
@@ -3245,7 +3248,7 @@
       <c r="P23" s="5">
         <v>14.51</v>
       </c>
-      <c r="Q23" s="19">
+      <c r="Q23" s="17">
         <v>3.66</v>
       </c>
       <c r="R23" s="10">
@@ -3255,46 +3258,46 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="T23" s="10">
-        <v>9.77</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="U23" s="10">
-        <v>1.06</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="V23" s="10">
         <v>0</v>
       </c>
       <c r="W23" s="10">
-        <v>7.31</v>
+        <v>7.3</v>
       </c>
       <c r="X23" s="10">
-        <v>91.88</v>
+        <v>91.9</v>
       </c>
       <c r="Y23" s="10">
-        <v>1.06</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="Z23" s="10">
         <v>0</v>
       </c>
       <c r="AA23" s="10">
-        <v>10.94</v>
+        <v>10.9</v>
       </c>
       <c r="AB23" s="10">
-        <v>91.88</v>
+        <v>91.9</v>
       </c>
       <c r="AC23" s="16">
-        <v>1.06</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="AD23" s="10">
         <v>0</v>
       </c>
       <c r="AE23" s="10">
-        <v>20.18</v>
+        <v>20.2</v>
       </c>
       <c r="AF23" s="10">
-        <v>91.88</v>
+        <v>91.9</v>
       </c>
       <c r="AG23" s="16">
-        <v>1.06</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="24" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -3323,19 +3326,19 @@
         <v>-83.205399999999997</v>
       </c>
       <c r="I24" s="4">
-        <v>65.33</v>
+        <v>65.3</v>
       </c>
       <c r="J24" s="4">
-        <v>464.92</v>
+        <v>464.9</v>
       </c>
       <c r="K24" s="5">
         <v>4.0999999999999996</v>
       </c>
       <c r="L24" s="4">
-        <v>5.54</v>
+        <v>3.6</v>
       </c>
       <c r="M24" s="4">
-        <v>10.76</v>
+        <v>10.8</v>
       </c>
       <c r="N24" s="5">
         <v>18.78</v>
@@ -3346,32 +3349,32 @@
       <c r="P24" s="5">
         <v>10.07</v>
       </c>
-      <c r="Q24" s="19">
+      <c r="Q24" s="17">
         <v>3.82</v>
       </c>
       <c r="R24" s="10">
         <v>0</v>
       </c>
       <c r="S24" s="10">
-        <v>3.74</v>
+        <v>3.7</v>
       </c>
       <c r="T24" s="10">
-        <v>2.4900000000000002</v>
+        <v>2.5</v>
       </c>
       <c r="U24" s="10">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="V24" s="10">
         <v>0</v>
       </c>
-      <c r="W24" s="10">
-        <v>4.99</v>
+      <c r="W24" s="14">
+        <v>5</v>
       </c>
       <c r="X24" s="10">
-        <v>57.13</v>
+        <v>57.1</v>
       </c>
       <c r="Y24" s="10">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="Z24" s="10">
         <v>0</v>
@@ -3380,22 +3383,22 @@
         <v>7.3</v>
       </c>
       <c r="AB24" s="10">
-        <v>57.82</v>
+        <v>57.8</v>
       </c>
       <c r="AC24" s="10">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="AD24" s="10">
         <v>0</v>
       </c>
       <c r="AE24" s="10">
-        <v>14.88</v>
+        <v>14.9</v>
       </c>
       <c r="AF24" s="10">
-        <v>57.82</v>
+        <v>57.8</v>
       </c>
       <c r="AG24" s="10">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="25" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -3424,19 +3427,19 @@
         <v>-83.212699999999998</v>
       </c>
       <c r="I25" s="4">
-        <v>9.08</v>
+        <v>9.1</v>
       </c>
       <c r="J25" s="4">
-        <v>471.17</v>
+        <v>471.2</v>
       </c>
       <c r="K25" s="5">
-        <v>3.27</v>
+        <v>3.3</v>
       </c>
       <c r="L25" s="4">
-        <v>2.38</v>
+        <v>0.2</v>
       </c>
       <c r="M25" s="4">
-        <v>0.92</v>
+        <v>0.9</v>
       </c>
       <c r="N25" s="5">
         <v>35.340000000000003</v>
@@ -3447,7 +3450,7 @@
       <c r="P25" s="5">
         <v>5.4</v>
       </c>
-      <c r="Q25" s="19">
+      <c r="Q25" s="17">
         <v>2.15</v>
       </c>
       <c r="R25" s="10">
@@ -3456,11 +3459,11 @@
       <c r="S25" s="10">
         <v>0</v>
       </c>
-      <c r="T25" s="15">
+      <c r="T25" s="14">
         <v>16.7</v>
       </c>
-      <c r="U25" s="10">
-        <v>22.99</v>
+      <c r="U25" s="14">
+        <v>23</v>
       </c>
       <c r="V25" s="10">
         <v>0</v>
@@ -3471,32 +3474,32 @@
       <c r="X25" s="15">
         <v>16.7</v>
       </c>
-      <c r="Y25" s="10">
-        <v>22.99</v>
+      <c r="Y25" s="14">
+        <v>23</v>
       </c>
       <c r="Z25" s="10">
         <v>0</v>
       </c>
       <c r="AA25" s="10">
-        <v>10.210000000000001</v>
-      </c>
-      <c r="AB25" s="15">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="AB25" s="14">
         <v>16.7</v>
       </c>
-      <c r="AC25" s="10">
-        <v>22.99</v>
+      <c r="AC25" s="14">
+        <v>23</v>
       </c>
       <c r="AD25" s="10">
         <v>0</v>
       </c>
       <c r="AE25" s="10">
-        <v>10.210000000000001</v>
-      </c>
-      <c r="AF25" s="17">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="AF25" s="37">
         <v>16.7</v>
       </c>
-      <c r="AG25" s="16">
-        <v>22.99</v>
+      <c r="AG25" s="37">
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -3530,14 +3533,14 @@
       <c r="J26" s="4">
         <v>461.4</v>
       </c>
-      <c r="K26" s="5">
-        <v>1.98</v>
-      </c>
-      <c r="L26" s="4">
-        <v>7.71</v>
+      <c r="K26" s="35">
+        <v>2</v>
+      </c>
+      <c r="L26" s="20">
+        <v>2</v>
       </c>
       <c r="M26" s="4">
-        <v>2.31</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="N26" s="5">
         <v>5.16</v>
@@ -3548,56 +3551,56 @@
       <c r="P26" s="5">
         <v>44.79</v>
       </c>
-      <c r="Q26" s="19">
+      <c r="Q26" s="17">
         <v>4.34</v>
       </c>
       <c r="R26" s="10">
         <v>0</v>
       </c>
-      <c r="S26" s="15">
+      <c r="S26" s="14">
         <v>1.5</v>
       </c>
       <c r="T26" s="10">
-        <v>13.79</v>
+        <v>13.8</v>
       </c>
       <c r="U26" s="10">
-        <v>0.77</v>
+        <v>0.8</v>
       </c>
       <c r="V26" s="10">
         <v>0</v>
       </c>
       <c r="W26" s="10">
-        <v>11.79</v>
+        <v>11.8</v>
       </c>
       <c r="X26" s="10">
-        <v>32.409999999999997</v>
+        <v>32.4</v>
       </c>
       <c r="Y26" s="10">
-        <v>0.77</v>
+        <v>0.8</v>
       </c>
       <c r="Z26" s="10">
         <v>0</v>
       </c>
       <c r="AA26" s="10">
-        <v>18.510000000000002</v>
+        <v>18.5</v>
       </c>
       <c r="AB26" s="10">
-        <v>32.409999999999997</v>
+        <v>32.4</v>
       </c>
       <c r="AC26" s="10">
-        <v>0.77</v>
+        <v>0.8</v>
       </c>
       <c r="AD26" s="10">
         <v>0</v>
       </c>
       <c r="AE26" s="10">
-        <v>20.170000000000002</v>
+        <v>20.2</v>
       </c>
       <c r="AF26" s="10">
         <v>100</v>
       </c>
       <c r="AG26" s="10">
-        <v>0.77</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="27" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -3632,13 +3635,13 @@
         <v>455.5</v>
       </c>
       <c r="K27" s="5">
-        <v>3.31</v>
+        <v>3.3</v>
       </c>
       <c r="L27" s="4">
-        <v>4.0599999999999996</v>
+        <v>0.1</v>
       </c>
       <c r="M27" s="4">
-        <v>12.17</v>
+        <v>12.2</v>
       </c>
       <c r="N27" s="5">
         <v>6.02</v>
@@ -3649,7 +3652,7 @@
       <c r="P27" s="5">
         <v>22.49</v>
       </c>
-      <c r="Q27" s="21">
+      <c r="Q27" s="19">
         <v>11.9</v>
       </c>
       <c r="R27" s="10">
@@ -3658,8 +3661,8 @@
       <c r="S27" s="10">
         <v>0</v>
       </c>
-      <c r="T27" s="10">
-        <v>2.02</v>
+      <c r="T27" s="14">
+        <v>2</v>
       </c>
       <c r="U27" s="10">
         <v>0</v>
@@ -3670,8 +3673,8 @@
       <c r="W27" s="10">
         <v>0</v>
       </c>
-      <c r="X27" s="10">
-        <v>2.02</v>
+      <c r="X27" s="14">
+        <v>2</v>
       </c>
       <c r="Y27" s="10">
         <v>0</v>
@@ -3682,8 +3685,8 @@
       <c r="AA27" s="10">
         <v>0</v>
       </c>
-      <c r="AB27" s="10">
-        <v>2.02</v>
+      <c r="AB27" s="14">
+        <v>2</v>
       </c>
       <c r="AC27" s="10">
         <v>0</v>
@@ -3727,19 +3730,19 @@
         <v>-83.322000000000003</v>
       </c>
       <c r="I28" s="4">
-        <v>16.02</v>
+        <v>16</v>
       </c>
       <c r="J28" s="4">
         <v>434.3</v>
       </c>
       <c r="K28" s="5">
-        <v>14.18</v>
+        <v>14.2</v>
       </c>
       <c r="L28" s="4">
         <v>3.08</v>
       </c>
       <c r="M28" s="4">
-        <v>2.23</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="N28" s="5">
         <v>34.99</v>
@@ -3750,7 +3753,7 @@
       <c r="P28" s="5">
         <v>7.86</v>
       </c>
-      <c r="Q28" s="19">
+      <c r="Q28" s="17">
         <v>6.26</v>
       </c>
       <c r="R28" s="10">
@@ -3768,11 +3771,11 @@
       <c r="V28" s="10">
         <v>0</v>
       </c>
-      <c r="W28" s="10">
-        <v>2.97</v>
+      <c r="W28" s="14">
+        <v>3</v>
       </c>
       <c r="X28" s="10">
-        <v>2.82</v>
+        <v>2.8</v>
       </c>
       <c r="Y28" s="10">
         <v>0</v>
@@ -3781,10 +3784,10 @@
         <v>23</v>
       </c>
       <c r="AA28" s="10">
-        <v>7.89</v>
+        <v>7.9</v>
       </c>
       <c r="AB28" s="10">
-        <v>2.82</v>
+        <v>2.8</v>
       </c>
       <c r="AC28" s="10">
         <v>0</v>
@@ -3792,10 +3795,10 @@
       <c r="AD28" s="14">
         <v>23</v>
       </c>
-      <c r="AE28" s="15">
+      <c r="AE28" s="14">
         <v>21.1</v>
       </c>
-      <c r="AF28" s="10">
+      <c r="AF28" s="14">
         <v>2.82</v>
       </c>
       <c r="AG28" s="10">
@@ -3828,19 +3831,19 @@
         <v>-83.3279</v>
       </c>
       <c r="I29" s="4">
-        <v>1.65</v>
+        <v>1.7</v>
       </c>
       <c r="J29" s="4">
         <v>455.2</v>
       </c>
       <c r="K29" s="5">
-        <v>13.11</v>
+        <v>13.1</v>
       </c>
       <c r="L29" s="4">
         <v>0.61</v>
       </c>
       <c r="M29" s="4">
-        <v>1.24</v>
+        <v>1.2</v>
       </c>
       <c r="N29" s="5">
         <v>66.790000000000006</v>
@@ -3851,7 +3854,7 @@
       <c r="P29" s="5">
         <v>0</v>
       </c>
-      <c r="Q29" s="19">
+      <c r="Q29" s="17">
         <v>6.71</v>
       </c>
       <c r="R29" s="10">
@@ -3870,7 +3873,7 @@
         <v>0</v>
       </c>
       <c r="W29" s="10">
-        <v>23.86</v>
+        <v>23.9</v>
       </c>
       <c r="X29" s="10">
         <v>0</v>
@@ -3882,7 +3885,7 @@
         <v>0</v>
       </c>
       <c r="AA29" s="10">
-        <v>23.86</v>
+        <v>23.9</v>
       </c>
       <c r="AB29" s="10">
         <v>0</v>
@@ -3894,7 +3897,7 @@
         <v>0</v>
       </c>
       <c r="AE29" s="10">
-        <v>23.86</v>
+        <v>23.9</v>
       </c>
       <c r="AF29" s="10">
         <v>0</v>
@@ -3929,16 +3932,16 @@
         <v>-83.8506</v>
       </c>
       <c r="I30" s="4">
-        <v>11.64</v>
+        <v>11.6</v>
       </c>
       <c r="J30" s="4">
-        <v>393.45</v>
+        <v>393.5</v>
       </c>
       <c r="K30" s="5">
-        <v>14.26</v>
+        <v>14.3</v>
       </c>
       <c r="L30" s="4">
-        <v>1.74</v>
+        <v>0.2</v>
       </c>
       <c r="M30" s="4">
         <v>3.9</v>
@@ -3952,7 +3955,7 @@
       <c r="P30" s="5">
         <v>0.46</v>
       </c>
-      <c r="Q30" s="19">
+      <c r="Q30" s="17">
         <v>2.67</v>
       </c>
       <c r="R30" s="10">
@@ -3962,7 +3965,7 @@
         <v>0</v>
       </c>
       <c r="T30" s="10">
-        <v>46.33</v>
+        <v>46.3</v>
       </c>
       <c r="U30" s="10">
         <v>0</v>
@@ -3971,10 +3974,10 @@
         <v>0</v>
       </c>
       <c r="W30" s="10">
-        <v>1.34</v>
+        <v>1.3</v>
       </c>
       <c r="X30" s="10">
-        <v>46.33</v>
+        <v>46.3</v>
       </c>
       <c r="Y30" s="10">
         <v>0</v>
@@ -3983,10 +3986,10 @@
         <v>0</v>
       </c>
       <c r="AA30" s="10">
-        <v>15.59</v>
+        <v>15.6</v>
       </c>
       <c r="AB30" s="10">
-        <v>46.33</v>
+        <v>46.3</v>
       </c>
       <c r="AC30" s="10">
         <v>0</v>
@@ -3995,9 +3998,9 @@
         <v>0</v>
       </c>
       <c r="AE30" s="10">
-        <v>24.16</v>
-      </c>
-      <c r="AF30" s="10">
+        <v>24.2</v>
+      </c>
+      <c r="AF30" s="14">
         <v>46.33</v>
       </c>
       <c r="AG30" s="10">
@@ -4033,16 +4036,16 @@
         <v>14.2</v>
       </c>
       <c r="J31" s="4">
-        <v>422.61</v>
+        <v>422.6</v>
       </c>
       <c r="K31" s="5">
-        <v>10.73</v>
+        <v>10.7</v>
       </c>
       <c r="L31" s="4">
-        <v>5.25</v>
+        <v>0.7</v>
       </c>
       <c r="M31" s="4">
-        <v>4.2300000000000004</v>
+        <v>4.2</v>
       </c>
       <c r="N31" s="5">
         <v>78.33</v>
@@ -4053,17 +4056,17 @@
       <c r="P31" s="5">
         <v>0.51</v>
       </c>
-      <c r="Q31" s="19">
+      <c r="Q31" s="17">
         <v>0.33</v>
       </c>
       <c r="R31" s="10">
         <v>0</v>
       </c>
       <c r="S31" s="10">
-        <v>6.11</v>
-      </c>
-      <c r="T31" s="15">
-        <v>44.54</v>
+        <v>6.1</v>
+      </c>
+      <c r="T31" s="14">
+        <v>44.5</v>
       </c>
       <c r="U31" s="10">
         <v>0</v>
@@ -4072,10 +4075,10 @@
         <v>0</v>
       </c>
       <c r="W31" s="10">
-        <v>25.11</v>
-      </c>
-      <c r="X31" s="15">
-        <v>44.54</v>
+        <v>25.1</v>
+      </c>
+      <c r="X31" s="14">
+        <v>44.5</v>
       </c>
       <c r="Y31" s="10">
         <v>0</v>
@@ -4084,10 +4087,10 @@
         <v>0</v>
       </c>
       <c r="AA31" s="10">
-        <v>25.11</v>
-      </c>
-      <c r="AB31" s="10">
-        <v>45.97</v>
+        <v>25.1</v>
+      </c>
+      <c r="AB31" s="14">
+        <v>46</v>
       </c>
       <c r="AC31" s="10">
         <v>0</v>
@@ -4096,10 +4099,10 @@
         <v>0</v>
       </c>
       <c r="AE31" s="10">
-        <v>35.94</v>
-      </c>
-      <c r="AF31" s="10">
-        <v>45.97</v>
+        <v>35.9</v>
+      </c>
+      <c r="AF31" s="14">
+        <v>46</v>
       </c>
       <c r="AG31" s="10">
         <v>0</v>
@@ -4129,290 +4132,290 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="27" x14ac:dyDescent="0.2">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="E2" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="F2" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="23" t="s">
+      <c r="G2" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="31" t="s">
+      <c r="H2" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="24" t="s">
+      <c r="I2" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="24" t="s">
+      <c r="J2" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="24" t="s">
-        <v>102</v>
+      <c r="K2" s="22" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="30">
+      <c r="D3" s="28">
         <v>106.8</v>
       </c>
-      <c r="E3" s="27">
+      <c r="E3" s="25">
         <v>13.3</v>
       </c>
-      <c r="F3" s="26">
+      <c r="F3" s="24">
         <v>3.3</v>
       </c>
-      <c r="G3" s="26">
+      <c r="G3" s="24">
         <v>12.4</v>
       </c>
-      <c r="H3" s="32">
+      <c r="H3" s="30">
         <v>28.5</v>
       </c>
-      <c r="I3" s="27">
+      <c r="I3" s="25">
         <v>53.3</v>
       </c>
-      <c r="J3" s="27">
+      <c r="J3" s="25">
         <v>4.8</v>
       </c>
-      <c r="K3" s="27">
+      <c r="K3" s="25">
         <v>3.4</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="30">
+      <c r="D4" s="28">
         <v>2.1</v>
       </c>
-      <c r="E4" s="27">
+      <c r="E4" s="25">
         <v>7.5</v>
       </c>
-      <c r="F4" s="26">
+      <c r="F4" s="24">
         <v>0.8</v>
       </c>
-      <c r="G4" s="26">
+      <c r="G4" s="24">
         <v>1.1000000000000001</v>
       </c>
-      <c r="H4" s="32">
+      <c r="H4" s="30">
         <v>20.8</v>
       </c>
-      <c r="I4" s="27">
+      <c r="I4" s="25">
         <v>39.700000000000003</v>
       </c>
-      <c r="J4" s="27">
+      <c r="J4" s="25">
         <v>16.899999999999999</v>
       </c>
-      <c r="K4" s="27">
+      <c r="K4" s="25">
         <v>14.3</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="30">
+      <c r="D5" s="28">
         <v>0.4</v>
       </c>
-      <c r="E5" s="27">
+      <c r="E5" s="25">
         <v>6.3</v>
       </c>
-      <c r="F5" s="26">
+      <c r="F5" s="24">
         <v>20.6</v>
       </c>
-      <c r="G5" s="26">
-        <v>0</v>
-      </c>
-      <c r="H5" s="32">
+      <c r="G5" s="24">
+        <v>0</v>
+      </c>
+      <c r="H5" s="30">
         <v>4.0999999999999996</v>
       </c>
-      <c r="I5" s="27">
+      <c r="I5" s="25">
         <v>55.3</v>
       </c>
-      <c r="J5" s="27">
+      <c r="J5" s="25">
         <v>19.399999999999999</v>
       </c>
-      <c r="K5" s="27">
+      <c r="K5" s="25">
         <v>12.7</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="33">
+      <c r="D6" s="31">
         <v>1.5</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="32">
         <v>4.9000000000000004</v>
       </c>
-      <c r="F6" s="35">
+      <c r="F6" s="33">
         <v>2.1</v>
       </c>
-      <c r="G6" s="26">
+      <c r="G6" s="24">
         <v>8.1</v>
       </c>
-      <c r="H6" s="36">
+      <c r="H6" s="34">
         <v>8.3000000000000007</v>
       </c>
-      <c r="I6" s="27">
+      <c r="I6" s="25">
         <v>39.700000000000003</v>
       </c>
-      <c r="J6" s="27">
+      <c r="J6" s="25">
         <v>15.9</v>
       </c>
-      <c r="K6" s="34">
+      <c r="K6" s="32">
         <v>17.899999999999999</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="30">
+      <c r="D7" s="28">
         <v>1.2</v>
       </c>
-      <c r="E7" s="27">
+      <c r="E7" s="25">
         <v>13.1</v>
       </c>
-      <c r="F7" s="35">
+      <c r="F7" s="33">
         <v>10</v>
       </c>
-      <c r="G7" s="26">
-        <v>0</v>
-      </c>
-      <c r="H7" s="36">
+      <c r="G7" s="24">
+        <v>0</v>
+      </c>
+      <c r="H7" s="34">
         <v>8</v>
       </c>
-      <c r="I7" s="27">
+      <c r="I7" s="25">
         <v>64.400000000000006</v>
       </c>
-      <c r="J7" s="27">
+      <c r="J7" s="25">
         <v>14.4</v>
       </c>
-      <c r="K7" s="27">
+      <c r="K7" s="25">
         <v>9.9</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="30">
+      <c r="D8" s="28">
         <v>1.7</v>
       </c>
-      <c r="E8" s="27">
+      <c r="E8" s="25">
         <v>13.1</v>
       </c>
-      <c r="F8" s="26">
+      <c r="F8" s="24">
         <v>0.6</v>
       </c>
-      <c r="G8" s="26">
+      <c r="G8" s="24">
         <v>1.2</v>
       </c>
-      <c r="H8" s="32">
+      <c r="H8" s="30">
         <v>66.8</v>
       </c>
-      <c r="I8" s="27">
+      <c r="I8" s="25">
         <v>20.7</v>
       </c>
-      <c r="J8" s="27">
-        <v>0</v>
-      </c>
-      <c r="K8" s="27">
+      <c r="J8" s="25">
+        <v>0</v>
+      </c>
+      <c r="K8" s="25">
         <v>6.7</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="30">
+      <c r="D9" s="28">
         <v>11.6</v>
       </c>
-      <c r="E9" s="27">
+      <c r="E9" s="25">
         <v>14.3</v>
       </c>
-      <c r="F9" s="26">
+      <c r="F9" s="24">
         <v>1.7</v>
       </c>
-      <c r="G9" s="35">
+      <c r="G9" s="33">
         <v>3.9</v>
       </c>
-      <c r="H9" s="36">
+      <c r="H9" s="34">
         <v>68.8</v>
       </c>
-      <c r="I9" s="27">
+      <c r="I9" s="25">
         <v>22.8</v>
       </c>
-      <c r="J9" s="27">
+      <c r="J9" s="25">
         <v>0.5</v>
       </c>
-      <c r="K9" s="27">
+      <c r="K9" s="25">
         <v>2.7</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="C10" s="28" t="s">
+      <c r="C10" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="33">
+      <c r="D10" s="31">
         <v>14.2</v>
       </c>
-      <c r="E10" s="27">
+      <c r="E10" s="25">
         <v>10.7</v>
       </c>
-      <c r="F10" s="26">
+      <c r="F10" s="24">
         <v>5.3</v>
       </c>
-      <c r="G10" s="26">
+      <c r="G10" s="24">
         <v>4.2</v>
       </c>
-      <c r="H10" s="32">
+      <c r="H10" s="30">
         <v>78.3</v>
       </c>
-      <c r="I10" s="27">
+      <c r="I10" s="25">
         <v>15.2</v>
       </c>
-      <c r="J10" s="27">
+      <c r="J10" s="25">
         <v>0.51</v>
       </c>
-      <c r="K10" s="27">
+      <c r="K10" s="25">
         <v>0.3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
upd - corrected WS 87 calculations
</commit_message>
<xml_diff>
--- a/Watershed_table_v1.xlsx
+++ b/Watershed_table_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/MW/2020 Trent University/R/Thesis Data/MSc_data_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{732DF53C-B433-4F48-9EA2-380D2A267CFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97701A74-E68A-5D4D-ABEC-7F825CE286F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9180" yWindow="680" windowWidth="29080" windowHeight="8440" xr2:uid="{3AD1715B-176F-3140-B9AE-F64F14EE2DEE}"/>
+    <workbookView xWindow="10560" yWindow="500" windowWidth="18160" windowHeight="9040" xr2:uid="{3AD1715B-176F-3140-B9AE-F64F14EE2DEE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -963,10 +963,10 @@
   <dimension ref="A1:AG31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="174" zoomScaleNormal="162" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="I15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J10" sqref="J10"/>
+      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
upd - adjusted graph to show g C /m^2/season. Excel mass load sheet updated too.
</commit_message>
<xml_diff>
--- a/Watershed_table_v1.xlsx
+++ b/Watershed_table_v1.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/MW/2020 Trent University/R/Thesis Data/MSc_data_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97701A74-E68A-5D4D-ABEC-7F825CE286F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FBD2D56-667D-E84A-91F5-46006C039A82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10560" yWindow="500" windowWidth="18160" windowHeight="9040" xr2:uid="{3AD1715B-176F-3140-B9AE-F64F14EE2DEE}"/>
+    <workbookView xWindow="15760" yWindow="500" windowWidth="22620" windowHeight="7740" xr2:uid="{3AD1715B-176F-3140-B9AE-F64F14EE2DEE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,6 +28,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -963,10 +965,10 @@
   <dimension ref="A1:AG31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="174" zoomScaleNormal="162" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="I15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="I25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomRight" activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2820,7 +2822,7 @@
       <c r="H19" s="4">
         <v>-83.142300000000006</v>
       </c>
-      <c r="I19" s="4">
+      <c r="I19" s="20">
         <v>46</v>
       </c>
       <c r="J19" s="4">

</xml_diff>

<commit_message>
upd - adjusted code for wetland plot (reflects the new percentages from Erika's FRI computation).
</commit_message>
<xml_diff>
--- a/Watershed_table_v1.xlsx
+++ b/Watershed_table_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/MW/2020 Trent University/R/Thesis Data/MSc_data_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FBD2D56-667D-E84A-91F5-46006C039A82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5DB0565-5CA9-2D40-BBB7-EAA42325984C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15760" yWindow="500" windowWidth="22620" windowHeight="7740" xr2:uid="{3AD1715B-176F-3140-B9AE-F64F14EE2DEE}"/>
+    <workbookView xWindow="22160" yWindow="760" windowWidth="10140" windowHeight="14440" xr2:uid="{3AD1715B-176F-3140-B9AE-F64F14EE2DEE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="105">
   <si>
     <t>Site name</t>
   </si>
@@ -371,6 +371,13 @@
   </si>
   <si>
     <t>20-year Abiotic Disturbance (%)</t>
+  </si>
+  <si>
+    <t>Productive
+Forest (%)</t>
+  </si>
+  <si>
+    <t>100.0*</t>
   </si>
 </sst>
 </file>
@@ -549,7 +556,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -587,13 +594,7 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -965,10 +966,10 @@
   <dimension ref="A1:AG31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="174" zoomScaleNormal="162" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="I25" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I14" sqref="I14"/>
+      <selection pane="bottomRight" activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1019,17 +1020,17 @@
       <c r="M1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="N1" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="O1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="P1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="Q1" s="7" t="s">
         <v>11</v>
-      </c>
-      <c r="Q1" s="9" t="s">
-        <v>89</v>
       </c>
       <c r="R1" s="9" t="s">
         <v>86</v>
@@ -1114,23 +1115,23 @@
       <c r="K2" s="5">
         <v>7.8</v>
       </c>
-      <c r="L2" s="20">
-        <v>0.5</v>
+      <c r="L2" s="18">
+        <v>6.7</v>
       </c>
       <c r="M2" s="4">
         <v>4.5</v>
       </c>
-      <c r="N2" s="5">
+      <c r="N2" s="4">
+        <v>88.2</v>
+      </c>
+      <c r="O2" s="5">
         <v>7.57</v>
       </c>
-      <c r="O2" s="5">
+      <c r="P2" s="5">
         <v>59.04</v>
       </c>
-      <c r="P2" s="5">
+      <c r="Q2" s="5">
         <v>12.43</v>
-      </c>
-      <c r="Q2" s="17">
-        <v>2.61</v>
       </c>
       <c r="R2" s="10">
         <v>0</v>
@@ -1207,7 +1208,7 @@
         <v>-84.764600000000002</v>
       </c>
       <c r="I3" s="4">
-        <v>30.6</v>
+        <v>44.1</v>
       </c>
       <c r="J3" s="4">
         <v>339.3</v>
@@ -1216,22 +1217,22 @@
         <v>12.2</v>
       </c>
       <c r="L3" s="4">
-        <v>0.9</v>
-      </c>
-      <c r="M3" s="20">
+        <v>0.8</v>
+      </c>
+      <c r="M3" s="18">
         <v>27</v>
       </c>
-      <c r="N3" s="5">
+      <c r="N3" s="18">
+        <v>69.400000000000006</v>
+      </c>
+      <c r="O3" s="5">
         <v>17.72</v>
       </c>
-      <c r="O3" s="5">
+      <c r="P3" s="5">
         <v>44.46</v>
       </c>
-      <c r="P3" s="5">
+      <c r="Q3" s="5">
         <v>3.61</v>
-      </c>
-      <c r="Q3" s="17">
-        <v>0.97</v>
       </c>
       <c r="R3" s="10">
         <v>0</v>
@@ -1317,22 +1318,22 @@
         <v>8.6</v>
       </c>
       <c r="L4" s="4">
-        <v>6.2</v>
+        <v>3.7</v>
       </c>
       <c r="M4" s="4">
         <v>12.7</v>
       </c>
-      <c r="N4" s="5">
+      <c r="N4" s="4">
+        <v>86.1</v>
+      </c>
+      <c r="O4" s="5">
         <v>23.18</v>
       </c>
-      <c r="O4" s="5">
+      <c r="P4" s="5">
         <v>56.92</v>
       </c>
-      <c r="P4" s="5">
+      <c r="Q4" s="5">
         <v>3.95</v>
-      </c>
-      <c r="Q4" s="17">
-        <v>1.46</v>
       </c>
       <c r="R4" s="10">
         <v>0</v>
@@ -1418,22 +1419,22 @@
         <v>13.3</v>
       </c>
       <c r="L5" s="4">
-        <v>3.3</v>
+        <v>3.1</v>
       </c>
       <c r="M5" s="4">
         <v>12.4</v>
       </c>
-      <c r="N5" s="5">
+      <c r="N5" s="4">
+        <v>93.9</v>
+      </c>
+      <c r="O5" s="5">
         <v>28.52</v>
       </c>
-      <c r="O5" s="5">
+      <c r="P5" s="5">
         <v>53.27</v>
       </c>
-      <c r="P5" s="5">
+      <c r="Q5" s="5">
         <v>4.8099999999999996</v>
-      </c>
-      <c r="Q5" s="17">
-        <v>3.44</v>
       </c>
       <c r="R5" s="10">
         <v>0</v>
@@ -1512,29 +1513,29 @@
       <c r="I6" s="4">
         <v>39.299999999999997</v>
       </c>
-      <c r="J6" s="20">
+      <c r="J6" s="18">
         <v>394.9</v>
       </c>
       <c r="K6" s="5">
         <v>12.2</v>
       </c>
-      <c r="L6" s="20">
-        <v>0.4</v>
+      <c r="L6" s="18">
+        <v>4</v>
       </c>
       <c r="M6" s="4">
         <v>3.7</v>
       </c>
-      <c r="N6" s="5">
+      <c r="N6" s="4">
+        <v>95.3</v>
+      </c>
+      <c r="O6" s="5">
         <v>18.52</v>
       </c>
-      <c r="O6" s="5">
+      <c r="P6" s="5">
         <v>66.86</v>
       </c>
-      <c r="P6" s="5">
+      <c r="Q6" s="5">
         <v>5.53</v>
-      </c>
-      <c r="Q6" s="17">
-        <v>1.48</v>
       </c>
       <c r="R6" s="10">
         <v>0</v>
@@ -1619,23 +1620,23 @@
       <c r="K7" s="5">
         <v>6.2</v>
       </c>
-      <c r="L7" s="4">
-        <v>7.8</v>
+      <c r="L7" s="18">
+        <v>3</v>
       </c>
       <c r="M7" s="4">
         <v>0.7</v>
       </c>
-      <c r="N7" s="5">
+      <c r="N7" s="4">
+        <v>92.2</v>
+      </c>
+      <c r="O7" s="5">
         <v>15.18</v>
       </c>
-      <c r="O7" s="5">
+      <c r="P7" s="5">
         <v>64.349999999999994</v>
       </c>
-      <c r="P7" s="5">
+      <c r="Q7" s="5">
         <v>5.1100000000000003</v>
-      </c>
-      <c r="Q7" s="17">
-        <v>3.87</v>
       </c>
       <c r="R7" s="10">
         <v>0</v>
@@ -1714,29 +1715,29 @@
       <c r="I8" s="4">
         <v>2.1</v>
       </c>
-      <c r="J8" s="20">
+      <c r="J8" s="18">
         <v>431</v>
       </c>
       <c r="K8" s="5">
         <v>7.5</v>
       </c>
       <c r="L8" s="4">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="M8" s="4">
         <v>1.1000000000000001</v>
       </c>
-      <c r="N8" s="5">
+      <c r="N8" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="O8" s="5">
         <v>20.83</v>
       </c>
-      <c r="O8" s="5">
+      <c r="P8" s="5">
         <v>39.65</v>
       </c>
-      <c r="P8" s="5">
+      <c r="Q8" s="5">
         <v>16.91</v>
-      </c>
-      <c r="Q8" s="17">
-        <v>14.34</v>
       </c>
       <c r="R8" s="10">
         <v>0</v>
@@ -1821,23 +1822,23 @@
       <c r="K9" s="5">
         <v>7.2</v>
       </c>
-      <c r="L9" s="20">
-        <v>11.6</v>
-      </c>
-      <c r="M9" s="20">
+      <c r="L9" s="18">
+        <v>10.1</v>
+      </c>
+      <c r="M9" s="18">
         <v>4.9000000000000004</v>
       </c>
       <c r="N9" s="18">
+        <v>88</v>
+      </c>
+      <c r="O9" s="17">
         <v>18.5</v>
       </c>
-      <c r="O9" s="5">
+      <c r="P9" s="5">
         <v>43.89</v>
       </c>
-      <c r="P9" s="5">
+      <c r="Q9" s="5">
         <v>7.61</v>
-      </c>
-      <c r="Q9" s="17">
-        <v>15.21</v>
       </c>
       <c r="R9" s="10">
         <v>0</v>
@@ -1923,22 +1924,22 @@
         <v>6.3</v>
       </c>
       <c r="L10" s="4">
-        <v>0.1</v>
+        <v>13.8</v>
       </c>
       <c r="M10" s="4">
         <v>0</v>
       </c>
-      <c r="N10" s="5">
+      <c r="N10" s="4">
+        <v>85.6</v>
+      </c>
+      <c r="O10" s="5">
         <v>4.17</v>
       </c>
-      <c r="O10" s="5">
+      <c r="P10" s="5">
         <v>55.31</v>
       </c>
-      <c r="P10" s="5">
+      <c r="Q10" s="5">
         <v>19.350000000000001</v>
-      </c>
-      <c r="Q10" s="17">
-        <v>12.69</v>
       </c>
       <c r="R10" s="10">
         <v>0</v>
@@ -2024,22 +2025,22 @@
         <v>4.5</v>
       </c>
       <c r="L11" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="M11" s="20">
+        <v>11.3</v>
+      </c>
+      <c r="M11" s="18">
         <v>5</v>
       </c>
-      <c r="N11" s="5">
+      <c r="N11" s="18">
+        <v>82.6</v>
+      </c>
+      <c r="O11" s="5">
         <v>2.44</v>
       </c>
-      <c r="O11" s="5">
+      <c r="P11" s="5">
         <v>60.56</v>
       </c>
-      <c r="P11" s="5">
+      <c r="Q11" s="5">
         <v>4.21</v>
-      </c>
-      <c r="Q11" s="17">
-        <v>17.64</v>
       </c>
       <c r="R11" s="10">
         <v>0</v>
@@ -2125,22 +2126,22 @@
         <v>4.5</v>
       </c>
       <c r="L12" s="4">
-        <v>1.8</v>
+        <v>5.9</v>
       </c>
       <c r="M12" s="4">
         <v>5.3</v>
       </c>
-      <c r="N12" s="5">
+      <c r="N12" s="4">
+        <v>89.7</v>
+      </c>
+      <c r="O12" s="5">
         <v>11.62</v>
       </c>
-      <c r="O12" s="5">
+      <c r="P12" s="5">
         <v>42.39</v>
       </c>
-      <c r="P12" s="5">
+      <c r="Q12" s="5">
         <v>18.12</v>
-      </c>
-      <c r="Q12" s="17">
-        <v>3.91</v>
       </c>
       <c r="R12" s="10">
         <v>0</v>
@@ -2226,22 +2227,22 @@
         <v>3.7</v>
       </c>
       <c r="L13" s="4">
-        <v>1.2</v>
+        <v>6.9</v>
       </c>
       <c r="M13" s="4">
         <v>32.700000000000003</v>
       </c>
-      <c r="N13" s="5">
+      <c r="N13" s="4">
+        <v>61.1</v>
+      </c>
+      <c r="O13" s="5">
         <v>3.26</v>
       </c>
-      <c r="O13" s="5">
+      <c r="P13" s="5">
         <v>28.56</v>
       </c>
-      <c r="P13" s="5">
+      <c r="Q13" s="5">
         <v>22.66</v>
-      </c>
-      <c r="Q13" s="17">
-        <v>4.62</v>
       </c>
       <c r="R13" s="10">
         <v>0</v>
@@ -2327,22 +2328,22 @@
         <v>5.5</v>
       </c>
       <c r="L14" s="4">
-        <v>0.6</v>
+        <v>3.9</v>
       </c>
       <c r="M14" s="4">
         <v>20.8</v>
       </c>
-      <c r="N14" s="5">
+      <c r="N14" s="4">
+        <v>76.3</v>
+      </c>
+      <c r="O14" s="5">
         <v>19.96</v>
       </c>
-      <c r="O14" s="5">
+      <c r="P14" s="5">
         <v>34.450000000000003</v>
       </c>
-      <c r="P14" s="5">
+      <c r="Q14" s="5">
         <v>8.15</v>
-      </c>
-      <c r="Q14" s="17">
-        <v>4.7699999999999996</v>
       </c>
       <c r="R14" s="10">
         <v>0</v>
@@ -2428,22 +2429,20 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="L15" s="4">
-        <v>7.6</v>
+        <v>7.5</v>
       </c>
       <c r="M15" s="4">
         <v>0.3</v>
       </c>
-      <c r="N15" s="5">
+      <c r="N15" s="4"/>
+      <c r="O15" s="5">
         <v>18.12</v>
       </c>
-      <c r="O15" s="5">
+      <c r="P15" s="5">
         <v>26.87</v>
       </c>
-      <c r="P15" s="5">
+      <c r="Q15" s="5">
         <v>35.92</v>
-      </c>
-      <c r="Q15" s="17">
-        <v>3.44</v>
       </c>
       <c r="R15" s="10">
         <v>0</v>
@@ -2529,22 +2528,20 @@
         <v>7.2</v>
       </c>
       <c r="L16" s="4">
-        <v>3.2</v>
+        <v>6.9</v>
       </c>
       <c r="M16" s="4">
         <v>2.2000000000000002</v>
       </c>
-      <c r="N16" s="5">
+      <c r="N16" s="4"/>
+      <c r="O16" s="5">
         <v>44.57</v>
       </c>
-      <c r="O16" s="5">
+      <c r="P16" s="5">
         <v>32.07</v>
       </c>
-      <c r="P16" s="5">
+      <c r="Q16" s="5">
         <v>14.62</v>
-      </c>
-      <c r="Q16" s="17">
-        <v>1.73</v>
       </c>
       <c r="R16" s="10">
         <v>0</v>
@@ -2629,23 +2626,23 @@
       <c r="K17" s="5">
         <v>3.8</v>
       </c>
-      <c r="L17" s="20">
-        <v>5</v>
+      <c r="L17" s="34">
+        <v>0</v>
       </c>
       <c r="M17" s="4">
         <v>0</v>
       </c>
-      <c r="N17" s="5">
-        <v>0</v>
+      <c r="N17" s="4">
+        <v>99.4</v>
       </c>
       <c r="O17" s="5">
+        <v>0</v>
+      </c>
+      <c r="P17" s="5">
         <v>77.599999999999994</v>
       </c>
-      <c r="P17" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="17">
-        <v>17.3</v>
+      <c r="Q17" s="5">
+        <v>0</v>
       </c>
       <c r="R17" s="10">
         <v>0</v>
@@ -2730,23 +2727,23 @@
       <c r="K18" s="5">
         <v>4.9000000000000004</v>
       </c>
-      <c r="L18" s="36">
-        <v>0</v>
+      <c r="L18" s="18">
+        <v>10.3</v>
       </c>
       <c r="M18" s="4">
         <v>8.1</v>
       </c>
-      <c r="N18" s="18">
+      <c r="N18" s="4">
+        <v>82.5</v>
+      </c>
+      <c r="O18" s="17">
         <v>8.3000000000000007</v>
       </c>
-      <c r="O18" s="5">
+      <c r="P18" s="5">
         <v>39.67</v>
       </c>
-      <c r="P18" s="5">
+      <c r="Q18" s="5">
         <v>15.94</v>
-      </c>
-      <c r="Q18" s="17">
-        <v>17.899999999999999</v>
       </c>
       <c r="R18" s="10">
         <v>0</v>
@@ -2822,7 +2819,7 @@
       <c r="H19" s="4">
         <v>-83.142300000000006</v>
       </c>
-      <c r="I19" s="20">
+      <c r="I19" s="18">
         <v>46</v>
       </c>
       <c r="J19" s="4">
@@ -2832,22 +2829,22 @@
         <v>12.1</v>
       </c>
       <c r="L19" s="4">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="M19" s="4">
         <v>9.4</v>
       </c>
-      <c r="N19" s="5">
+      <c r="N19" s="4">
+        <v>87.4</v>
+      </c>
+      <c r="O19" s="5">
         <v>18.63</v>
       </c>
-      <c r="O19" s="5">
+      <c r="P19" s="5">
         <v>48.56</v>
       </c>
-      <c r="P19" s="5">
+      <c r="Q19" s="5">
         <v>11.72</v>
-      </c>
-      <c r="Q19" s="17">
-        <v>8.19</v>
       </c>
       <c r="R19" s="10">
         <v>0</v>
@@ -2932,23 +2929,23 @@
       <c r="K20" s="5">
         <v>13.1</v>
       </c>
-      <c r="L20" s="20">
-        <v>10</v>
+      <c r="L20" s="18">
+        <v>5.4</v>
       </c>
       <c r="M20" s="4">
         <v>0</v>
       </c>
-      <c r="N20" s="5">
+      <c r="N20" s="4">
+        <v>93.6</v>
+      </c>
+      <c r="O20" s="5">
         <v>7.97</v>
       </c>
-      <c r="O20" s="5">
+      <c r="P20" s="5">
         <v>64.430000000000007</v>
       </c>
-      <c r="P20" s="5">
+      <c r="Q20" s="5">
         <v>14.38</v>
-      </c>
-      <c r="Q20" s="17">
-        <v>9.92</v>
       </c>
       <c r="R20" s="10">
         <v>0</v>
@@ -3034,22 +3031,22 @@
         <v>9.9</v>
       </c>
       <c r="L21" s="4">
-        <v>0.7</v>
+        <v>3.6</v>
       </c>
       <c r="M21" s="4">
         <v>1.9</v>
       </c>
-      <c r="N21" s="5">
+      <c r="N21" s="4">
+        <v>93.2</v>
+      </c>
+      <c r="O21" s="5">
         <v>37.369999999999997</v>
       </c>
-      <c r="O21" s="5">
+      <c r="P21" s="5">
         <v>39.1</v>
       </c>
-      <c r="P21" s="5">
+      <c r="Q21" s="5">
         <v>12.77</v>
-      </c>
-      <c r="Q21" s="17">
-        <v>4.1399999999999997</v>
       </c>
       <c r="R21" s="10">
         <v>0</v>
@@ -3135,22 +3132,22 @@
         <v>3.6</v>
       </c>
       <c r="L22" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="M22" s="20">
+        <v>14.2</v>
+      </c>
+      <c r="M22" s="18">
         <v>5</v>
       </c>
-      <c r="N22" s="5">
+      <c r="N22" s="18">
+        <v>79.900000000000006</v>
+      </c>
+      <c r="O22" s="5">
         <v>1.04</v>
       </c>
-      <c r="O22" s="5">
+      <c r="P22" s="5">
         <v>56.69</v>
       </c>
-      <c r="P22" s="5">
+      <c r="Q22" s="5">
         <v>20.49</v>
-      </c>
-      <c r="Q22" s="17">
-        <v>0.61</v>
       </c>
       <c r="R22" s="10">
         <v>0</v>
@@ -3226,32 +3223,32 @@
       <c r="H23" s="4">
         <v>-83.200699999999998</v>
       </c>
-      <c r="I23" s="20">
+      <c r="I23" s="18">
         <v>36</v>
       </c>
       <c r="J23" s="4">
         <v>482.3</v>
       </c>
-      <c r="K23" s="35">
+      <c r="K23" s="33">
         <v>6</v>
       </c>
       <c r="L23" s="4">
-        <v>1.3</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="M23" s="4">
         <v>4.7</v>
       </c>
-      <c r="N23" s="5">
+      <c r="N23" s="4">
+        <v>89.7</v>
+      </c>
+      <c r="O23" s="5">
         <v>28.98</v>
       </c>
-      <c r="O23" s="5">
+      <c r="P23" s="5">
         <v>40.24</v>
       </c>
-      <c r="P23" s="5">
+      <c r="Q23" s="5">
         <v>14.51</v>
-      </c>
-      <c r="Q23" s="17">
-        <v>3.66</v>
       </c>
       <c r="R23" s="10">
         <v>0</v>
@@ -3337,22 +3334,22 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="L24" s="4">
-        <v>3.6</v>
+        <v>3.7</v>
       </c>
       <c r="M24" s="4">
         <v>10.8</v>
       </c>
-      <c r="N24" s="5">
+      <c r="N24" s="4">
+        <v>85.5</v>
+      </c>
+      <c r="O24" s="5">
         <v>18.78</v>
       </c>
-      <c r="O24" s="5">
+      <c r="P24" s="5">
         <v>43.99</v>
       </c>
-      <c r="P24" s="5">
+      <c r="Q24" s="5">
         <v>10.07</v>
-      </c>
-      <c r="Q24" s="17">
-        <v>3.82</v>
       </c>
       <c r="R24" s="10">
         <v>0</v>
@@ -3438,22 +3435,22 @@
         <v>3.3</v>
       </c>
       <c r="L25" s="4">
-        <v>0.2</v>
+        <v>2.4</v>
       </c>
       <c r="M25" s="4">
         <v>0.9</v>
       </c>
-      <c r="N25" s="5">
+      <c r="N25" s="4">
+        <v>94.1</v>
+      </c>
+      <c r="O25" s="5">
         <v>35.340000000000003</v>
       </c>
-      <c r="O25" s="5">
+      <c r="P25" s="5">
         <v>40.51</v>
       </c>
-      <c r="P25" s="5">
+      <c r="Q25" s="5">
         <v>5.4</v>
-      </c>
-      <c r="Q25" s="17">
-        <v>2.15</v>
       </c>
       <c r="R25" s="10">
         <v>0</v>
@@ -3497,10 +3494,10 @@
       <c r="AE25" s="10">
         <v>10.199999999999999</v>
       </c>
-      <c r="AF25" s="37">
+      <c r="AF25" s="35">
         <v>16.7</v>
       </c>
-      <c r="AG25" s="37">
+      <c r="AG25" s="35">
         <v>23</v>
       </c>
     </row>
@@ -3535,26 +3532,26 @@
       <c r="J26" s="4">
         <v>461.4</v>
       </c>
-      <c r="K26" s="35">
+      <c r="K26" s="33">
         <v>2</v>
       </c>
-      <c r="L26" s="20">
-        <v>2</v>
+      <c r="L26" s="18">
+        <v>2.4</v>
       </c>
       <c r="M26" s="4">
         <v>2.2999999999999998</v>
       </c>
-      <c r="N26" s="5">
+      <c r="N26" s="4">
+        <v>91.2</v>
+      </c>
+      <c r="O26" s="5">
         <v>5.16</v>
       </c>
-      <c r="O26" s="5">
+      <c r="P26" s="5">
         <v>28.16</v>
       </c>
-      <c r="P26" s="5">
+      <c r="Q26" s="5">
         <v>44.79</v>
-      </c>
-      <c r="Q26" s="17">
-        <v>4.34</v>
       </c>
       <c r="R26" s="10">
         <v>0</v>
@@ -3640,22 +3637,22 @@
         <v>3.3</v>
       </c>
       <c r="L27" s="4">
-        <v>0.1</v>
+        <v>6.9</v>
       </c>
       <c r="M27" s="4">
         <v>12.2</v>
       </c>
-      <c r="N27" s="5">
+      <c r="N27" s="4">
+        <v>74.900000000000006</v>
+      </c>
+      <c r="O27" s="5">
         <v>6.02</v>
       </c>
-      <c r="O27" s="5">
+      <c r="P27" s="5">
         <v>42.38</v>
       </c>
-      <c r="P27" s="5">
+      <c r="Q27" s="5">
         <v>22.49</v>
-      </c>
-      <c r="Q27" s="19">
-        <v>11.9</v>
       </c>
       <c r="R27" s="10">
         <v>0</v>
@@ -3731,7 +3728,7 @@
       <c r="H28" s="5">
         <v>-83.322000000000003</v>
       </c>
-      <c r="I28" s="4">
+      <c r="I28" s="18">
         <v>16</v>
       </c>
       <c r="J28" s="4">
@@ -3741,22 +3738,22 @@
         <v>14.2</v>
       </c>
       <c r="L28" s="4">
-        <v>3.08</v>
+        <v>4.2</v>
       </c>
       <c r="M28" s="4">
         <v>2.2000000000000002</v>
       </c>
-      <c r="N28" s="5">
+      <c r="N28" s="4">
+        <v>92.9</v>
+      </c>
+      <c r="O28" s="5">
         <v>34.99</v>
       </c>
-      <c r="O28" s="5">
+      <c r="P28" s="5">
         <v>41.92</v>
       </c>
-      <c r="P28" s="5">
+      <c r="Q28" s="5">
         <v>7.86</v>
-      </c>
-      <c r="Q28" s="17">
-        <v>6.26</v>
       </c>
       <c r="R28" s="10">
         <v>0</v>
@@ -3842,22 +3839,22 @@
         <v>13.1</v>
       </c>
       <c r="L29" s="4">
-        <v>0.61</v>
+        <v>2.9</v>
       </c>
       <c r="M29" s="4">
         <v>1.2</v>
       </c>
-      <c r="N29" s="5">
+      <c r="N29" s="18">
+        <v>94</v>
+      </c>
+      <c r="O29" s="5">
         <v>66.790000000000006</v>
       </c>
-      <c r="O29" s="5">
+      <c r="P29" s="5">
         <v>20.65</v>
       </c>
-      <c r="P29" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q29" s="17">
-        <v>6.71</v>
+      <c r="Q29" s="5">
+        <v>0</v>
       </c>
       <c r="R29" s="10">
         <v>0</v>
@@ -3943,22 +3940,22 @@
         <v>14.3</v>
       </c>
       <c r="L30" s="4">
-        <v>0.2</v>
+        <v>1.6</v>
       </c>
       <c r="M30" s="4">
         <v>3.9</v>
       </c>
-      <c r="N30" s="5">
+      <c r="N30" s="4">
+        <v>94.9</v>
+      </c>
+      <c r="O30" s="5">
         <v>68.8</v>
       </c>
-      <c r="O30" s="5">
+      <c r="P30" s="5">
         <v>22.82</v>
       </c>
-      <c r="P30" s="5">
+      <c r="Q30" s="5">
         <v>0.46</v>
-      </c>
-      <c r="Q30" s="17">
-        <v>2.67</v>
       </c>
       <c r="R30" s="10">
         <v>0</v>
@@ -4044,22 +4041,22 @@
         <v>10.7</v>
       </c>
       <c r="L31" s="4">
-        <v>0.7</v>
+        <v>4.3</v>
       </c>
       <c r="M31" s="4">
         <v>4.2</v>
       </c>
-      <c r="N31" s="5">
+      <c r="N31" s="18">
+        <v>93</v>
+      </c>
+      <c r="O31" s="5">
         <v>78.33</v>
       </c>
-      <c r="O31" s="5">
+      <c r="P31" s="5">
         <v>15.17</v>
       </c>
-      <c r="P31" s="5">
+      <c r="Q31" s="5">
         <v>0.51</v>
-      </c>
-      <c r="Q31" s="17">
-        <v>0.33</v>
       </c>
       <c r="R31" s="10">
         <v>0</v>
@@ -4134,290 +4131,290 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="27" x14ac:dyDescent="0.2">
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="21" t="s">
+      <c r="G2" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="29" t="s">
+      <c r="H2" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="22" t="s">
+      <c r="I2" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="22" t="s">
+      <c r="J2" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="22" t="s">
+      <c r="K2" s="20" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="28">
+      <c r="D3" s="26">
         <v>106.8</v>
       </c>
-      <c r="E3" s="25">
+      <c r="E3" s="23">
         <v>13.3</v>
       </c>
-      <c r="F3" s="24">
+      <c r="F3" s="22">
         <v>3.3</v>
       </c>
-      <c r="G3" s="24">
+      <c r="G3" s="22">
         <v>12.4</v>
       </c>
-      <c r="H3" s="30">
+      <c r="H3" s="28">
         <v>28.5</v>
       </c>
-      <c r="I3" s="25">
+      <c r="I3" s="23">
         <v>53.3</v>
       </c>
-      <c r="J3" s="25">
+      <c r="J3" s="23">
         <v>4.8</v>
       </c>
-      <c r="K3" s="25">
+      <c r="K3" s="23">
         <v>3.4</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="28">
+      <c r="D4" s="26">
         <v>2.1</v>
       </c>
-      <c r="E4" s="25">
+      <c r="E4" s="23">
         <v>7.5</v>
       </c>
-      <c r="F4" s="24">
+      <c r="F4" s="22">
         <v>0.8</v>
       </c>
-      <c r="G4" s="24">
+      <c r="G4" s="22">
         <v>1.1000000000000001</v>
       </c>
-      <c r="H4" s="30">
+      <c r="H4" s="28">
         <v>20.8</v>
       </c>
-      <c r="I4" s="25">
+      <c r="I4" s="23">
         <v>39.700000000000003</v>
       </c>
-      <c r="J4" s="25">
+      <c r="J4" s="23">
         <v>16.899999999999999</v>
       </c>
-      <c r="K4" s="25">
+      <c r="K4" s="23">
         <v>14.3</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="28">
+      <c r="D5" s="26">
         <v>0.4</v>
       </c>
-      <c r="E5" s="25">
+      <c r="E5" s="23">
         <v>6.3</v>
       </c>
-      <c r="F5" s="24">
+      <c r="F5" s="22">
         <v>20.6</v>
       </c>
-      <c r="G5" s="24">
-        <v>0</v>
-      </c>
-      <c r="H5" s="30">
+      <c r="G5" s="22">
+        <v>0</v>
+      </c>
+      <c r="H5" s="28">
         <v>4.0999999999999996</v>
       </c>
-      <c r="I5" s="25">
+      <c r="I5" s="23">
         <v>55.3</v>
       </c>
-      <c r="J5" s="25">
+      <c r="J5" s="23">
         <v>19.399999999999999</v>
       </c>
-      <c r="K5" s="25">
+      <c r="K5" s="23">
         <v>12.7</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="31">
+      <c r="D6" s="29">
         <v>1.5</v>
       </c>
-      <c r="E6" s="32">
+      <c r="E6" s="30">
         <v>4.9000000000000004</v>
       </c>
-      <c r="F6" s="33">
+      <c r="F6" s="31">
         <v>2.1</v>
       </c>
-      <c r="G6" s="24">
+      <c r="G6" s="22">
         <v>8.1</v>
       </c>
-      <c r="H6" s="34">
+      <c r="H6" s="32">
         <v>8.3000000000000007</v>
       </c>
-      <c r="I6" s="25">
+      <c r="I6" s="23">
         <v>39.700000000000003</v>
       </c>
-      <c r="J6" s="25">
+      <c r="J6" s="23">
         <v>15.9</v>
       </c>
-      <c r="K6" s="32">
+      <c r="K6" s="30">
         <v>17.899999999999999</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="C7" s="24" t="s">
+      <c r="C7" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="28">
+      <c r="D7" s="26">
         <v>1.2</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="23">
         <v>13.1</v>
       </c>
-      <c r="F7" s="33">
+      <c r="F7" s="31">
         <v>10</v>
       </c>
-      <c r="G7" s="24">
-        <v>0</v>
-      </c>
-      <c r="H7" s="34">
+      <c r="G7" s="22">
+        <v>0</v>
+      </c>
+      <c r="H7" s="32">
         <v>8</v>
       </c>
-      <c r="I7" s="25">
+      <c r="I7" s="23">
         <v>64.400000000000006</v>
       </c>
-      <c r="J7" s="25">
+      <c r="J7" s="23">
         <v>14.4</v>
       </c>
-      <c r="K7" s="25">
+      <c r="K7" s="23">
         <v>9.9</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="C8" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="28">
+      <c r="D8" s="26">
         <v>1.7</v>
       </c>
-      <c r="E8" s="25">
+      <c r="E8" s="23">
         <v>13.1</v>
       </c>
-      <c r="F8" s="24">
+      <c r="F8" s="22">
         <v>0.6</v>
       </c>
-      <c r="G8" s="24">
+      <c r="G8" s="22">
         <v>1.2</v>
       </c>
-      <c r="H8" s="30">
+      <c r="H8" s="28">
         <v>66.8</v>
       </c>
-      <c r="I8" s="25">
+      <c r="I8" s="23">
         <v>20.7</v>
       </c>
-      <c r="J8" s="25">
-        <v>0</v>
-      </c>
-      <c r="K8" s="25">
+      <c r="J8" s="23">
+        <v>0</v>
+      </c>
+      <c r="K8" s="23">
         <v>6.7</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="C9" s="26" t="s">
+      <c r="C9" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="28">
+      <c r="D9" s="26">
         <v>11.6</v>
       </c>
-      <c r="E9" s="25">
+      <c r="E9" s="23">
         <v>14.3</v>
       </c>
-      <c r="F9" s="24">
+      <c r="F9" s="22">
         <v>1.7</v>
       </c>
-      <c r="G9" s="33">
+      <c r="G9" s="31">
         <v>3.9</v>
       </c>
-      <c r="H9" s="34">
+      <c r="H9" s="32">
         <v>68.8</v>
       </c>
-      <c r="I9" s="25">
+      <c r="I9" s="23">
         <v>22.8</v>
       </c>
-      <c r="J9" s="25">
+      <c r="J9" s="23">
         <v>0.5</v>
       </c>
-      <c r="K9" s="25">
+      <c r="K9" s="23">
         <v>2.7</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="C10" s="26" t="s">
+      <c r="C10" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="31">
+      <c r="D10" s="29">
         <v>14.2</v>
       </c>
-      <c r="E10" s="25">
+      <c r="E10" s="23">
         <v>10.7</v>
       </c>
-      <c r="F10" s="24">
+      <c r="F10" s="22">
         <v>5.3</v>
       </c>
-      <c r="G10" s="24">
+      <c r="G10" s="22">
         <v>4.2</v>
       </c>
-      <c r="H10" s="30">
+      <c r="H10" s="28">
         <v>78.3</v>
       </c>
-      <c r="I10" s="25">
+      <c r="I10" s="23">
         <v>15.2</v>
       </c>
-      <c r="J10" s="25">
+      <c r="J10" s="23">
         <v>0.51</v>
       </c>
-      <c r="K10" s="25">
+      <c r="K10" s="23">
         <v>0.3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
upd - used new ws table values to update all DOC concentration plots and create all DOC export plots.
</commit_message>
<xml_diff>
--- a/Watershed_table_v1.xlsx
+++ b/Watershed_table_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/MW/2020 Trent University/R/Thesis Data/MSc_data_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5DB0565-5CA9-2D40-BBB7-EAA42325984C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E993AC8E-A5DA-5F41-B96B-C049DCA6D58E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22160" yWindow="760" windowWidth="10140" windowHeight="14440" xr2:uid="{3AD1715B-176F-3140-B9AE-F64F14EE2DEE}"/>
+    <workbookView xWindow="21180" yWindow="500" windowWidth="16900" windowHeight="14780" xr2:uid="{3AD1715B-176F-3140-B9AE-F64F14EE2DEE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="104">
   <si>
     <t>Site name</t>
   </si>
@@ -373,11 +373,7 @@
     <t>20-year Abiotic Disturbance (%)</t>
   </si>
   <si>
-    <t>Productive
-Forest (%)</t>
-  </si>
-  <si>
-    <t>100.0*</t>
+    <t>Total Productive Forest (%)</t>
   </si>
 </sst>
 </file>
@@ -556,7 +552,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -594,9 +590,6 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -966,17 +959,19 @@
   <dimension ref="A1:AG31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="174" zoomScaleNormal="162" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L2" sqref="L2"/>
+      <selection pane="bottomRight" activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="7.6640625" customWidth="1"/>
     <col min="2" max="2" width="14.83203125" customWidth="1"/>
     <col min="4" max="4" width="13.6640625" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
+    <col min="14" max="14" width="11.6640625" customWidth="1"/>
     <col min="22" max="22" width="10.5" style="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1115,23 +1110,21 @@
       <c r="K2" s="5">
         <v>7.8</v>
       </c>
-      <c r="L2" s="18">
+      <c r="L2" s="17">
         <v>6.7</v>
       </c>
-      <c r="M2" s="4">
-        <v>4.5</v>
+      <c r="M2" s="17">
+        <v>3</v>
       </c>
       <c r="N2" s="4">
         <v>88.2</v>
       </c>
       <c r="O2" s="5">
-        <v>7.57</v>
-      </c>
-      <c r="P2" s="5">
-        <v>59.04</v>
-      </c>
-      <c r="Q2" s="5">
-        <v>12.43</v>
+        <v>37.6</v>
+      </c>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="32">
+        <v>39</v>
       </c>
       <c r="R2" s="10">
         <v>0</v>
@@ -1219,20 +1212,18 @@
       <c r="L3" s="4">
         <v>0.8</v>
       </c>
-      <c r="M3" s="18">
-        <v>27</v>
-      </c>
-      <c r="N3" s="18">
+      <c r="M3" s="17">
+        <v>17.8</v>
+      </c>
+      <c r="N3" s="17">
         <v>69.400000000000006</v>
       </c>
       <c r="O3" s="5">
-        <v>17.72</v>
-      </c>
-      <c r="P3" s="5">
-        <v>44.46</v>
-      </c>
+        <v>41.6</v>
+      </c>
+      <c r="P3" s="5"/>
       <c r="Q3" s="5">
-        <v>3.61</v>
+        <v>56.1</v>
       </c>
       <c r="R3" s="10">
         <v>0</v>
@@ -1321,19 +1312,17 @@
         <v>3.7</v>
       </c>
       <c r="M4" s="4">
-        <v>12.7</v>
+        <v>8.4</v>
       </c>
       <c r="N4" s="4">
         <v>86.1</v>
       </c>
       <c r="O4" s="5">
-        <v>23.18</v>
-      </c>
-      <c r="P4" s="5">
-        <v>56.92</v>
-      </c>
-      <c r="Q4" s="5">
-        <v>3.95</v>
+        <v>42.6</v>
+      </c>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="32">
+        <v>57</v>
       </c>
       <c r="R4" s="10">
         <v>0</v>
@@ -1422,19 +1411,17 @@
         <v>3.1</v>
       </c>
       <c r="M5" s="4">
-        <v>12.4</v>
+        <v>6.1</v>
       </c>
       <c r="N5" s="4">
         <v>93.9</v>
       </c>
       <c r="O5" s="5">
-        <v>28.52</v>
-      </c>
-      <c r="P5" s="5">
-        <v>53.27</v>
-      </c>
+        <v>56.5</v>
+      </c>
+      <c r="P5" s="5"/>
       <c r="Q5" s="5">
-        <v>4.8099999999999996</v>
+        <v>38.1</v>
       </c>
       <c r="R5" s="10">
         <v>0</v>
@@ -1513,29 +1500,27 @@
       <c r="I6" s="4">
         <v>39.299999999999997</v>
       </c>
-      <c r="J6" s="18">
+      <c r="J6" s="17">
         <v>394.9</v>
       </c>
       <c r="K6" s="5">
         <v>12.2</v>
       </c>
-      <c r="L6" s="18">
+      <c r="L6" s="17">
         <v>4</v>
       </c>
       <c r="M6" s="4">
-        <v>3.7</v>
+        <v>2.9</v>
       </c>
       <c r="N6" s="4">
         <v>95.3</v>
       </c>
       <c r="O6" s="5">
-        <v>18.52</v>
-      </c>
-      <c r="P6" s="5">
-        <v>66.86</v>
-      </c>
+        <v>55.7</v>
+      </c>
+      <c r="P6" s="5"/>
       <c r="Q6" s="5">
-        <v>5.53</v>
+        <v>39.799999999999997</v>
       </c>
       <c r="R6" s="10">
         <v>0</v>
@@ -1620,23 +1605,21 @@
       <c r="K7" s="5">
         <v>6.2</v>
       </c>
-      <c r="L7" s="18">
+      <c r="L7" s="17">
         <v>3</v>
       </c>
       <c r="M7" s="4">
-        <v>0.7</v>
+        <v>2.4</v>
       </c>
       <c r="N7" s="4">
         <v>92.2</v>
       </c>
       <c r="O7" s="5">
-        <v>15.18</v>
-      </c>
-      <c r="P7" s="5">
-        <v>64.349999999999994</v>
-      </c>
+        <v>57.2</v>
+      </c>
+      <c r="P7" s="5"/>
       <c r="Q7" s="5">
-        <v>5.1100000000000003</v>
+        <v>27.7</v>
       </c>
       <c r="R7" s="10">
         <v>0</v>
@@ -1715,7 +1698,7 @@
       <c r="I8" s="4">
         <v>2.1</v>
       </c>
-      <c r="J8" s="18">
+      <c r="J8" s="17">
         <v>431</v>
       </c>
       <c r="K8" s="5">
@@ -1725,19 +1708,17 @@
         <v>0.1</v>
       </c>
       <c r="M8" s="4">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="N8" s="4" t="s">
-        <v>104</v>
+        <v>0.8</v>
+      </c>
+      <c r="N8" s="17">
+        <v>100</v>
       </c>
       <c r="O8" s="5">
-        <v>20.83</v>
-      </c>
-      <c r="P8" s="5">
-        <v>39.65</v>
-      </c>
+        <v>36.700000000000003</v>
+      </c>
+      <c r="P8" s="5"/>
       <c r="Q8" s="5">
-        <v>16.91</v>
+        <v>56.6</v>
       </c>
       <c r="R8" s="10">
         <v>0</v>
@@ -1822,23 +1803,21 @@
       <c r="K9" s="5">
         <v>7.2</v>
       </c>
-      <c r="L9" s="18">
+      <c r="L9" s="17">
         <v>10.1</v>
       </c>
-      <c r="M9" s="18">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="N9" s="18">
+      <c r="M9" s="17">
+        <v>0</v>
+      </c>
+      <c r="N9" s="17">
         <v>88</v>
       </c>
-      <c r="O9" s="17">
-        <v>18.5</v>
-      </c>
-      <c r="P9" s="5">
-        <v>43.89</v>
-      </c>
+      <c r="O9" s="32">
+        <v>35.1</v>
+      </c>
+      <c r="P9" s="5"/>
       <c r="Q9" s="5">
-        <v>7.61</v>
+        <v>64.599999999999994</v>
       </c>
       <c r="R9" s="10">
         <v>0</v>
@@ -1932,14 +1911,12 @@
       <c r="N10" s="4">
         <v>85.6</v>
       </c>
-      <c r="O10" s="5">
-        <v>4.17</v>
-      </c>
-      <c r="P10" s="5">
-        <v>55.31</v>
-      </c>
+      <c r="O10" s="32">
+        <v>39</v>
+      </c>
+      <c r="P10" s="5"/>
       <c r="Q10" s="5">
-        <v>19.350000000000001</v>
+        <v>58.4</v>
       </c>
       <c r="R10" s="10">
         <v>0</v>
@@ -2027,20 +2004,18 @@
       <c r="L11" s="4">
         <v>11.3</v>
       </c>
-      <c r="M11" s="18">
-        <v>5</v>
-      </c>
-      <c r="N11" s="18">
+      <c r="M11" s="17">
+        <v>5.5</v>
+      </c>
+      <c r="N11" s="17">
         <v>82.6</v>
       </c>
       <c r="O11" s="5">
-        <v>2.44</v>
-      </c>
-      <c r="P11" s="5">
-        <v>60.56</v>
-      </c>
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="P11" s="5"/>
       <c r="Q11" s="5">
-        <v>4.21</v>
+        <v>30.8</v>
       </c>
       <c r="R11" s="10">
         <v>0</v>
@@ -2129,19 +2104,17 @@
         <v>5.9</v>
       </c>
       <c r="M12" s="4">
-        <v>5.3</v>
+        <v>4.3</v>
       </c>
       <c r="N12" s="4">
         <v>89.7</v>
       </c>
       <c r="O12" s="5">
-        <v>11.62</v>
-      </c>
-      <c r="P12" s="5">
-        <v>42.39</v>
-      </c>
+        <v>22.3</v>
+      </c>
+      <c r="P12" s="5"/>
       <c r="Q12" s="5">
-        <v>18.12</v>
+        <v>41.7</v>
       </c>
       <c r="R12" s="10">
         <v>0</v>
@@ -2230,19 +2203,17 @@
         <v>6.9</v>
       </c>
       <c r="M13" s="4">
-        <v>32.700000000000003</v>
+        <v>29.5</v>
       </c>
       <c r="N13" s="4">
         <v>61.1</v>
       </c>
       <c r="O13" s="5">
-        <v>3.26</v>
-      </c>
-      <c r="P13" s="5">
-        <v>28.56</v>
-      </c>
+        <v>23.7</v>
+      </c>
+      <c r="P13" s="5"/>
       <c r="Q13" s="5">
-        <v>22.66</v>
+        <v>53.4</v>
       </c>
       <c r="R13" s="10">
         <v>0</v>
@@ -2331,19 +2302,17 @@
         <v>3.9</v>
       </c>
       <c r="M14" s="4">
-        <v>20.8</v>
+        <v>17.3</v>
       </c>
       <c r="N14" s="4">
         <v>76.3</v>
       </c>
-      <c r="O14" s="5">
-        <v>19.96</v>
-      </c>
-      <c r="P14" s="5">
-        <v>34.450000000000003</v>
-      </c>
+      <c r="O14" s="32">
+        <v>41</v>
+      </c>
+      <c r="P14" s="5"/>
       <c r="Q14" s="5">
-        <v>8.15</v>
+        <v>57.1</v>
       </c>
       <c r="R14" s="10">
         <v>0</v>
@@ -2432,17 +2401,17 @@
         <v>7.5</v>
       </c>
       <c r="M15" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="N15" s="4"/>
+        <v>0.6</v>
+      </c>
+      <c r="N15" s="4">
+        <v>88.2</v>
+      </c>
       <c r="O15" s="5">
-        <v>18.12</v>
-      </c>
-      <c r="P15" s="5">
-        <v>26.87</v>
-      </c>
+        <v>27.4</v>
+      </c>
+      <c r="P15" s="5"/>
       <c r="Q15" s="5">
-        <v>35.92</v>
+        <v>72.599999999999994</v>
       </c>
       <c r="R15" s="10">
         <v>0</v>
@@ -2531,17 +2500,17 @@
         <v>6.9</v>
       </c>
       <c r="M16" s="4">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="N16" s="4"/>
+        <v>0.4</v>
+      </c>
+      <c r="N16" s="4">
+        <v>91.9</v>
+      </c>
       <c r="O16" s="5">
-        <v>44.57</v>
-      </c>
-      <c r="P16" s="5">
-        <v>32.07</v>
-      </c>
+        <v>53.1</v>
+      </c>
+      <c r="P16" s="5"/>
       <c r="Q16" s="5">
-        <v>14.62</v>
+        <v>46.2</v>
       </c>
       <c r="R16" s="10">
         <v>0</v>
@@ -2626,7 +2595,7 @@
       <c r="K17" s="5">
         <v>3.8</v>
       </c>
-      <c r="L17" s="34">
+      <c r="L17" s="33">
         <v>0</v>
       </c>
       <c r="M17" s="4">
@@ -2636,13 +2605,11 @@
         <v>99.4</v>
       </c>
       <c r="O17" s="5">
-        <v>0</v>
-      </c>
-      <c r="P17" s="5">
-        <v>77.599999999999994</v>
-      </c>
+        <v>34.4</v>
+      </c>
+      <c r="P17" s="5"/>
       <c r="Q17" s="5">
-        <v>0</v>
+        <v>42.3</v>
       </c>
       <c r="R17" s="10">
         <v>0</v>
@@ -2727,23 +2694,21 @@
       <c r="K18" s="5">
         <v>4.9000000000000004</v>
       </c>
-      <c r="L18" s="18">
+      <c r="L18" s="17">
         <v>10.3</v>
       </c>
       <c r="M18" s="4">
-        <v>8.1</v>
+        <v>6.1</v>
       </c>
       <c r="N18" s="4">
         <v>82.5</v>
       </c>
-      <c r="O18" s="17">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="P18" s="5">
-        <v>39.67</v>
-      </c>
+      <c r="O18" s="32">
+        <v>43.8</v>
+      </c>
+      <c r="P18" s="5"/>
       <c r="Q18" s="5">
-        <v>15.94</v>
+        <v>39.5</v>
       </c>
       <c r="R18" s="10">
         <v>0</v>
@@ -2819,7 +2784,7 @@
       <c r="H19" s="4">
         <v>-83.142300000000006</v>
       </c>
-      <c r="I19" s="18">
+      <c r="I19" s="17">
         <v>46</v>
       </c>
       <c r="J19" s="4">
@@ -2832,19 +2797,17 @@
         <v>2.5</v>
       </c>
       <c r="M19" s="4">
-        <v>9.4</v>
+        <v>7.3</v>
       </c>
       <c r="N19" s="4">
         <v>87.4</v>
       </c>
       <c r="O19" s="5">
-        <v>18.63</v>
-      </c>
-      <c r="P19" s="5">
-        <v>48.56</v>
-      </c>
+        <v>59.1</v>
+      </c>
+      <c r="P19" s="5"/>
       <c r="Q19" s="5">
-        <v>11.72</v>
+        <v>10.3</v>
       </c>
       <c r="R19" s="10">
         <v>0</v>
@@ -2929,23 +2892,21 @@
       <c r="K20" s="5">
         <v>13.1</v>
       </c>
-      <c r="L20" s="18">
+      <c r="L20" s="17">
         <v>5.4</v>
       </c>
       <c r="M20" s="4">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="N20" s="4">
         <v>93.6</v>
       </c>
       <c r="O20" s="5">
-        <v>7.97</v>
-      </c>
-      <c r="P20" s="5">
-        <v>64.430000000000007</v>
-      </c>
-      <c r="Q20" s="5">
-        <v>14.38</v>
+        <v>51.6</v>
+      </c>
+      <c r="P20" s="5"/>
+      <c r="Q20" s="32">
+        <v>13</v>
       </c>
       <c r="R20" s="10">
         <v>0</v>
@@ -3039,14 +3000,12 @@
       <c r="N21" s="4">
         <v>93.2</v>
       </c>
-      <c r="O21" s="5">
-        <v>37.369999999999997</v>
-      </c>
-      <c r="P21" s="5">
-        <v>39.1</v>
-      </c>
+      <c r="O21" s="32">
+        <v>57</v>
+      </c>
+      <c r="P21" s="5"/>
       <c r="Q21" s="5">
-        <v>12.77</v>
+        <v>10.6</v>
       </c>
       <c r="R21" s="10">
         <v>0</v>
@@ -3134,20 +3093,18 @@
       <c r="L22" s="4">
         <v>14.2</v>
       </c>
-      <c r="M22" s="18">
-        <v>5</v>
-      </c>
-      <c r="N22" s="18">
+      <c r="M22" s="17">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="N22" s="17">
         <v>79.900000000000006</v>
       </c>
       <c r="O22" s="5">
-        <v>1.04</v>
-      </c>
-      <c r="P22" s="5">
-        <v>56.69</v>
-      </c>
+        <v>48.4</v>
+      </c>
+      <c r="P22" s="5"/>
       <c r="Q22" s="5">
-        <v>20.49</v>
+        <v>31.3</v>
       </c>
       <c r="R22" s="10">
         <v>0</v>
@@ -3223,32 +3180,30 @@
       <c r="H23" s="4">
         <v>-83.200699999999998</v>
       </c>
-      <c r="I23" s="18">
+      <c r="I23" s="17">
         <v>36</v>
       </c>
       <c r="J23" s="4">
         <v>482.3</v>
       </c>
-      <c r="K23" s="33">
+      <c r="K23" s="32">
         <v>6</v>
       </c>
       <c r="L23" s="4">
         <v>4.9000000000000004</v>
       </c>
       <c r="M23" s="4">
-        <v>4.7</v>
+        <v>3.8</v>
       </c>
       <c r="N23" s="4">
         <v>89.7</v>
       </c>
       <c r="O23" s="5">
-        <v>28.98</v>
-      </c>
-      <c r="P23" s="5">
-        <v>40.24</v>
-      </c>
+        <v>48.9</v>
+      </c>
+      <c r="P23" s="5"/>
       <c r="Q23" s="5">
-        <v>14.51</v>
+        <v>40.4</v>
       </c>
       <c r="R23" s="10">
         <v>0</v>
@@ -3337,19 +3292,17 @@
         <v>3.7</v>
       </c>
       <c r="M24" s="4">
-        <v>10.8</v>
+        <v>9.5</v>
       </c>
       <c r="N24" s="4">
         <v>85.5</v>
       </c>
       <c r="O24" s="5">
-        <v>18.78</v>
-      </c>
-      <c r="P24" s="5">
-        <v>43.99</v>
-      </c>
+        <v>49.2</v>
+      </c>
+      <c r="P24" s="5"/>
       <c r="Q24" s="5">
-        <v>10.07</v>
+        <v>29.8</v>
       </c>
       <c r="R24" s="10">
         <v>0</v>
@@ -3438,19 +3391,17 @@
         <v>2.4</v>
       </c>
       <c r="M25" s="4">
-        <v>0.9</v>
+        <v>0.7</v>
       </c>
       <c r="N25" s="4">
         <v>94.1</v>
       </c>
       <c r="O25" s="5">
-        <v>35.340000000000003</v>
-      </c>
-      <c r="P25" s="5">
-        <v>40.51</v>
-      </c>
+        <v>45.8</v>
+      </c>
+      <c r="P25" s="5"/>
       <c r="Q25" s="5">
-        <v>5.4</v>
+        <v>32.700000000000003</v>
       </c>
       <c r="R25" s="10">
         <v>0</v>
@@ -3494,10 +3445,10 @@
       <c r="AE25" s="10">
         <v>10.199999999999999</v>
       </c>
-      <c r="AF25" s="35">
+      <c r="AF25" s="34">
         <v>16.7</v>
       </c>
-      <c r="AG25" s="35">
+      <c r="AG25" s="34">
         <v>23</v>
       </c>
     </row>
@@ -3532,26 +3483,24 @@
       <c r="J26" s="4">
         <v>461.4</v>
       </c>
-      <c r="K26" s="33">
+      <c r="K26" s="32">
         <v>2</v>
       </c>
-      <c r="L26" s="18">
+      <c r="L26" s="17">
         <v>2.4</v>
       </c>
       <c r="M26" s="4">
-        <v>2.2999999999999998</v>
+        <v>1.8</v>
       </c>
       <c r="N26" s="4">
         <v>91.2</v>
       </c>
       <c r="O26" s="5">
-        <v>5.16</v>
-      </c>
-      <c r="P26" s="5">
-        <v>28.16</v>
-      </c>
+        <v>25.7</v>
+      </c>
+      <c r="P26" s="5"/>
       <c r="Q26" s="5">
-        <v>44.79</v>
+        <v>53.9</v>
       </c>
       <c r="R26" s="10">
         <v>0</v>
@@ -3640,19 +3589,17 @@
         <v>6.9</v>
       </c>
       <c r="M27" s="4">
-        <v>12.2</v>
+        <v>9.6</v>
       </c>
       <c r="N27" s="4">
         <v>74.900000000000006</v>
       </c>
       <c r="O27" s="5">
-        <v>6.02</v>
-      </c>
-      <c r="P27" s="5">
-        <v>42.38</v>
-      </c>
+        <v>38.5</v>
+      </c>
+      <c r="P27" s="5"/>
       <c r="Q27" s="5">
-        <v>22.49</v>
+        <v>14.9</v>
       </c>
       <c r="R27" s="10">
         <v>0</v>
@@ -3728,7 +3675,7 @@
       <c r="H28" s="5">
         <v>-83.322000000000003</v>
       </c>
-      <c r="I28" s="18">
+      <c r="I28" s="17">
         <v>16</v>
       </c>
       <c r="J28" s="4">
@@ -3741,19 +3688,17 @@
         <v>4.2</v>
       </c>
       <c r="M28" s="4">
-        <v>2.2000000000000002</v>
+        <v>1.4</v>
       </c>
       <c r="N28" s="4">
         <v>92.9</v>
       </c>
       <c r="O28" s="5">
-        <v>34.99</v>
-      </c>
-      <c r="P28" s="5">
-        <v>41.92</v>
-      </c>
+        <v>36.299999999999997</v>
+      </c>
+      <c r="P28" s="5"/>
       <c r="Q28" s="5">
-        <v>7.86</v>
+        <v>32.4</v>
       </c>
       <c r="R28" s="10">
         <v>0</v>
@@ -3842,19 +3787,17 @@
         <v>2.9</v>
       </c>
       <c r="M29" s="4">
-        <v>1.2</v>
-      </c>
-      <c r="N29" s="18">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="N29" s="17">
         <v>94</v>
       </c>
       <c r="O29" s="5">
-        <v>66.790000000000006</v>
-      </c>
-      <c r="P29" s="5">
-        <v>20.65</v>
-      </c>
+        <v>76.5</v>
+      </c>
+      <c r="P29" s="5"/>
       <c r="Q29" s="5">
-        <v>0</v>
+        <v>19.8</v>
       </c>
       <c r="R29" s="10">
         <v>0</v>
@@ -3942,20 +3885,18 @@
       <c r="L30" s="4">
         <v>1.6</v>
       </c>
-      <c r="M30" s="4">
-        <v>3.9</v>
+      <c r="M30" s="17">
+        <v>3</v>
       </c>
       <c r="N30" s="4">
         <v>94.9</v>
       </c>
       <c r="O30" s="5">
-        <v>68.8</v>
-      </c>
-      <c r="P30" s="5">
-        <v>22.82</v>
-      </c>
+        <v>46.9</v>
+      </c>
+      <c r="P30" s="5"/>
       <c r="Q30" s="5">
-        <v>0.46</v>
+        <v>28.9</v>
       </c>
       <c r="R30" s="10">
         <v>0</v>
@@ -4044,19 +3985,17 @@
         <v>4.3</v>
       </c>
       <c r="M31" s="4">
-        <v>4.2</v>
-      </c>
-      <c r="N31" s="18">
+        <v>2.1</v>
+      </c>
+      <c r="N31" s="17">
         <v>93</v>
       </c>
       <c r="O31" s="5">
-        <v>78.33</v>
-      </c>
-      <c r="P31" s="5">
-        <v>15.17</v>
-      </c>
+        <v>52.9</v>
+      </c>
+      <c r="P31" s="5"/>
       <c r="Q31" s="5">
-        <v>0.51</v>
+        <v>28.4</v>
       </c>
       <c r="R31" s="10">
         <v>0</v>
@@ -4131,290 +4070,290 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="27" x14ac:dyDescent="0.2">
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="27" t="s">
+      <c r="H2" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="20" t="s">
+      <c r="J2" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="20" t="s">
+      <c r="K2" s="19" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="26">
+      <c r="D3" s="25">
         <v>106.8</v>
       </c>
-      <c r="E3" s="23">
+      <c r="E3" s="22">
         <v>13.3</v>
       </c>
-      <c r="F3" s="22">
+      <c r="F3" s="21">
         <v>3.3</v>
       </c>
-      <c r="G3" s="22">
+      <c r="G3" s="21">
         <v>12.4</v>
       </c>
-      <c r="H3" s="28">
+      <c r="H3" s="27">
         <v>28.5</v>
       </c>
-      <c r="I3" s="23">
+      <c r="I3" s="22">
         <v>53.3</v>
       </c>
-      <c r="J3" s="23">
+      <c r="J3" s="22">
         <v>4.8</v>
       </c>
-      <c r="K3" s="23">
+      <c r="K3" s="22">
         <v>3.4</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="26">
+      <c r="D4" s="25">
         <v>2.1</v>
       </c>
-      <c r="E4" s="23">
+      <c r="E4" s="22">
         <v>7.5</v>
       </c>
-      <c r="F4" s="22">
+      <c r="F4" s="21">
         <v>0.8</v>
       </c>
-      <c r="G4" s="22">
+      <c r="G4" s="21">
         <v>1.1000000000000001</v>
       </c>
-      <c r="H4" s="28">
+      <c r="H4" s="27">
         <v>20.8</v>
       </c>
-      <c r="I4" s="23">
+      <c r="I4" s="22">
         <v>39.700000000000003</v>
       </c>
-      <c r="J4" s="23">
+      <c r="J4" s="22">
         <v>16.899999999999999</v>
       </c>
-      <c r="K4" s="23">
+      <c r="K4" s="22">
         <v>14.3</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="26">
+      <c r="D5" s="25">
         <v>0.4</v>
       </c>
-      <c r="E5" s="23">
+      <c r="E5" s="22">
         <v>6.3</v>
       </c>
-      <c r="F5" s="22">
+      <c r="F5" s="21">
         <v>20.6</v>
       </c>
-      <c r="G5" s="22">
-        <v>0</v>
-      </c>
-      <c r="H5" s="28">
+      <c r="G5" s="21">
+        <v>0</v>
+      </c>
+      <c r="H5" s="27">
         <v>4.0999999999999996</v>
       </c>
-      <c r="I5" s="23">
+      <c r="I5" s="22">
         <v>55.3</v>
       </c>
-      <c r="J5" s="23">
+      <c r="J5" s="22">
         <v>19.399999999999999</v>
       </c>
-      <c r="K5" s="23">
+      <c r="K5" s="22">
         <v>12.7</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="29">
+      <c r="D6" s="28">
         <v>1.5</v>
       </c>
-      <c r="E6" s="30">
+      <c r="E6" s="29">
         <v>4.9000000000000004</v>
       </c>
-      <c r="F6" s="31">
+      <c r="F6" s="30">
         <v>2.1</v>
       </c>
-      <c r="G6" s="22">
+      <c r="G6" s="21">
         <v>8.1</v>
       </c>
-      <c r="H6" s="32">
+      <c r="H6" s="31">
         <v>8.3000000000000007</v>
       </c>
-      <c r="I6" s="23">
+      <c r="I6" s="22">
         <v>39.700000000000003</v>
       </c>
-      <c r="J6" s="23">
+      <c r="J6" s="22">
         <v>15.9</v>
       </c>
-      <c r="K6" s="30">
+      <c r="K6" s="29">
         <v>17.899999999999999</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="26">
+      <c r="D7" s="25">
         <v>1.2</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="22">
         <v>13.1</v>
       </c>
-      <c r="F7" s="31">
+      <c r="F7" s="30">
         <v>10</v>
       </c>
-      <c r="G7" s="22">
-        <v>0</v>
-      </c>
-      <c r="H7" s="32">
+      <c r="G7" s="21">
+        <v>0</v>
+      </c>
+      <c r="H7" s="31">
         <v>8</v>
       </c>
-      <c r="I7" s="23">
+      <c r="I7" s="22">
         <v>64.400000000000006</v>
       </c>
-      <c r="J7" s="23">
+      <c r="J7" s="22">
         <v>14.4</v>
       </c>
-      <c r="K7" s="23">
+      <c r="K7" s="22">
         <v>9.9</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="26">
+      <c r="D8" s="25">
         <v>1.7</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="22">
         <v>13.1</v>
       </c>
-      <c r="F8" s="22">
+      <c r="F8" s="21">
         <v>0.6</v>
       </c>
-      <c r="G8" s="22">
+      <c r="G8" s="21">
         <v>1.2</v>
       </c>
-      <c r="H8" s="28">
+      <c r="H8" s="27">
         <v>66.8</v>
       </c>
-      <c r="I8" s="23">
+      <c r="I8" s="22">
         <v>20.7</v>
       </c>
-      <c r="J8" s="23">
-        <v>0</v>
-      </c>
-      <c r="K8" s="23">
+      <c r="J8" s="22">
+        <v>0</v>
+      </c>
+      <c r="K8" s="22">
         <v>6.7</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="26">
+      <c r="D9" s="25">
         <v>11.6</v>
       </c>
-      <c r="E9" s="23">
+      <c r="E9" s="22">
         <v>14.3</v>
       </c>
-      <c r="F9" s="22">
+      <c r="F9" s="21">
         <v>1.7</v>
       </c>
-      <c r="G9" s="31">
+      <c r="G9" s="30">
         <v>3.9</v>
       </c>
-      <c r="H9" s="32">
+      <c r="H9" s="31">
         <v>68.8</v>
       </c>
-      <c r="I9" s="23">
+      <c r="I9" s="22">
         <v>22.8</v>
       </c>
-      <c r="J9" s="23">
+      <c r="J9" s="22">
         <v>0.5</v>
       </c>
-      <c r="K9" s="23">
+      <c r="K9" s="22">
         <v>2.7</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="29">
+      <c r="D10" s="28">
         <v>14.2</v>
       </c>
-      <c r="E10" s="23">
+      <c r="E10" s="22">
         <v>10.7</v>
       </c>
-      <c r="F10" s="22">
+      <c r="F10" s="21">
         <v>5.3</v>
       </c>
-      <c r="G10" s="22">
+      <c r="G10" s="21">
         <v>4.2</v>
       </c>
-      <c r="H10" s="28">
+      <c r="H10" s="27">
         <v>78.3</v>
       </c>
-      <c r="I10" s="23">
+      <c r="I10" s="22">
         <v>15.2</v>
       </c>
-      <c r="J10" s="23">
+      <c r="J10" s="22">
         <v>0.51</v>
       </c>
-      <c r="K10" s="23">
+      <c r="K10" s="22">
         <v>0.3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
upd - created script for doc characteristics - mean, sd, coeff of variance and updated sheet 2 of watershed table to have table 1 - DOC characteristics...
</commit_message>
<xml_diff>
--- a/Watershed_table_v1.xlsx
+++ b/Watershed_table_v1.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/MW/2020 Trent University/R/Thesis Data/MSc_data_analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Matt 1/Desktop/2020 Trent University/R/Thesis Data/MSc_data_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E993AC8E-A5DA-5F41-B96B-C049DCA6D58E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{443ACC28-9208-F64A-B2DB-44C0C70C274C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21180" yWindow="500" windowWidth="16900" windowHeight="14780" xr2:uid="{3AD1715B-176F-3140-B9AE-F64F14EE2DEE}"/>
+    <workbookView xWindow="-580" yWindow="500" windowWidth="16580" windowHeight="17500" activeTab="1" xr2:uid="{3AD1715B-176F-3140-B9AE-F64F14EE2DEE}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Master_watershed_table_v1.00" sheetId="1" r:id="rId1"/>
+    <sheet name="Table 1.  DOC  characteristics" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="107">
   <si>
     <t>Site name</t>
   </si>
@@ -374,6 +375,15 @@
   </si>
   <si>
     <t>Total Productive Forest (%)</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>Standard Deviation</t>
+  </si>
+  <si>
+    <t>Coefficient of Variation</t>
   </si>
 </sst>
 </file>
@@ -552,7 +562,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -642,6 +652,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -660,7 +673,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -948,7 +961,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -958,11 +971,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB97E4CB-EAC5-A646-BEC3-C9E17C7337B6}">
   <dimension ref="A1:AG31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="174" zoomScaleNormal="162" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="174" zoomScaleNormal="162" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H1" sqref="H1:H1048576"/>
+      <selection pane="bottomRight" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4052,6 +4065,642 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5381714B-05BA-204C-BC88-34B6CCB1BFF8}">
+  <dimension ref="A1:F31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F32" sqref="F32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="35" t="s">
+        <v>104</v>
+      </c>
+      <c r="E1" s="35" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1" s="35" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="10">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="E2" s="10">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="F2" s="10">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="10">
+        <v>3.4</v>
+      </c>
+      <c r="E3" s="10">
+        <v>0.8</v>
+      </c>
+      <c r="F3" s="10">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="10">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="E4" s="14">
+        <v>1</v>
+      </c>
+      <c r="F4" s="10">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="10">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="E5" s="10">
+        <v>1.2</v>
+      </c>
+      <c r="F5" s="10">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="10">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="E6" s="14">
+        <v>1</v>
+      </c>
+      <c r="F6" s="10">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="10">
+        <v>14.3</v>
+      </c>
+      <c r="E7" s="14">
+        <v>2</v>
+      </c>
+      <c r="F7" s="10">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="10">
+        <v>11.5</v>
+      </c>
+      <c r="E8" s="10">
+        <v>5.4</v>
+      </c>
+      <c r="F8" s="10">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="10">
+        <v>16.8</v>
+      </c>
+      <c r="E9" s="10">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="F9" s="10">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="10">
+        <v>6.1</v>
+      </c>
+      <c r="E10" s="10">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F10" s="10">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="10">
+        <v>7.4</v>
+      </c>
+      <c r="E11" s="10">
+        <v>3.1</v>
+      </c>
+      <c r="F11" s="10">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="10">
+        <v>7.4</v>
+      </c>
+      <c r="E12" s="10">
+        <v>3.4</v>
+      </c>
+      <c r="F12" s="10">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="10">
+        <v>6.8</v>
+      </c>
+      <c r="E13" s="10">
+        <v>3.7</v>
+      </c>
+      <c r="F13" s="10">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="10">
+        <v>5.4</v>
+      </c>
+      <c r="E14" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="F14" s="10">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="10">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="E15" s="10">
+        <v>3.3</v>
+      </c>
+      <c r="F15" s="10">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="10">
+        <v>14.5</v>
+      </c>
+      <c r="E16" s="10">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="F16" s="10">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="10">
+        <v>27.7</v>
+      </c>
+      <c r="E17" s="10">
+        <v>7.4</v>
+      </c>
+      <c r="F17" s="10">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="10">
+        <v>10.3</v>
+      </c>
+      <c r="E18" s="10">
+        <v>0.4</v>
+      </c>
+      <c r="F18" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="10">
+        <v>3.9</v>
+      </c>
+      <c r="E19" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="F19" s="10">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="10">
+        <v>11.1</v>
+      </c>
+      <c r="E20" s="10">
+        <v>1.6</v>
+      </c>
+      <c r="F20" s="10">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" s="10">
+        <v>9.6</v>
+      </c>
+      <c r="E21" s="10">
+        <v>1.9</v>
+      </c>
+      <c r="F21" s="10">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" s="10">
+        <v>15.8</v>
+      </c>
+      <c r="E22" s="10">
+        <v>2.8</v>
+      </c>
+      <c r="F22" s="10">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" s="10">
+        <v>14.6</v>
+      </c>
+      <c r="E23" s="14">
+        <v>2</v>
+      </c>
+      <c r="F23" s="10">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24" s="10">
+        <v>6.6</v>
+      </c>
+      <c r="E24" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="F24" s="10">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D25" s="10">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="E25" s="10">
+        <v>1.5</v>
+      </c>
+      <c r="F25" s="10">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26" s="10">
+        <v>10.4</v>
+      </c>
+      <c r="E26" s="10">
+        <v>1.4</v>
+      </c>
+      <c r="F26" s="10">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" s="14">
+        <v>3.6</v>
+      </c>
+      <c r="E27" s="10">
+        <v>1.2</v>
+      </c>
+      <c r="F27" s="10">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D28" s="10">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="E28" s="10">
+        <v>1.3</v>
+      </c>
+      <c r="F28" s="10">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D29" s="10">
+        <v>13.7</v>
+      </c>
+      <c r="E29" s="10">
+        <v>1.5</v>
+      </c>
+      <c r="F29" s="10">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D30" s="10">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="E30" s="10">
+        <v>2.1</v>
+      </c>
+      <c r="F30" s="10">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D31" s="10">
+        <v>7.5</v>
+      </c>
+      <c r="E31" s="10">
+        <v>1.5</v>
+      </c>
+      <c r="F31" s="10">
+        <v>0.2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{191690F3-C00A-624F-AD30-A957AF041456}">
   <dimension ref="B2:K10"/>
   <sheetViews>

</xml_diff>

<commit_message>
upd - started script for mean DOC multiple regression.
</commit_message>
<xml_diff>
--- a/Watershed_table_v1.xlsx
+++ b/Watershed_table_v1.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Matt 1/Desktop/2020 Trent University/R/Thesis Data/MSc_data_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2365E30-8A7E-1F43-96DD-56408D09A924}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1651C69-EAC3-734F-801B-8E6FA57DAAD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="27140" windowHeight="17120" activeTab="1" xr2:uid="{3AD1715B-176F-3140-B9AE-F64F14EE2DEE}"/>
+    <workbookView xWindow="1820" yWindow="1740" windowWidth="27500" windowHeight="17500" xr2:uid="{3AD1715B-176F-3140-B9AE-F64F14EE2DEE}"/>
   </bookViews>
   <sheets>
     <sheet name="Master_watershed_table_v1.00" sheetId="1" r:id="rId1"/>
     <sheet name="Table 1.  DOC  characteristics" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Table 2. Euclidean distance" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="138">
   <si>
     <t>Site name</t>
   </si>
@@ -332,9 +332,6 @@
     <t>5-year Insect Disturbance (%)</t>
   </si>
   <si>
-    <t>Sparse Forest (%)</t>
-  </si>
-  <si>
     <t>5-year Abiotic Disturbance (%)</t>
   </si>
   <si>
@@ -384,6 +381,102 @@
   </si>
   <si>
     <t>Coefficient of Variation</t>
+  </si>
+  <si>
+    <t>pair</t>
+  </si>
+  <si>
+    <t>site.pair</t>
+  </si>
+  <si>
+    <t>M1-I1</t>
+  </si>
+  <si>
+    <t>I1-H1</t>
+  </si>
+  <si>
+    <t>H1-M2</t>
+  </si>
+  <si>
+    <t>M2-I2</t>
+  </si>
+  <si>
+    <t>I2-I3</t>
+  </si>
+  <si>
+    <t>I3-M3</t>
+  </si>
+  <si>
+    <t>M3-I4</t>
+  </si>
+  <si>
+    <t>I4-I5</t>
+  </si>
+  <si>
+    <t>I5-I6</t>
+  </si>
+  <si>
+    <t>I6-M4</t>
+  </si>
+  <si>
+    <t>M4-M5</t>
+  </si>
+  <si>
+    <t>M5-C1</t>
+  </si>
+  <si>
+    <t>C1-C2</t>
+  </si>
+  <si>
+    <t>C2-C3</t>
+  </si>
+  <si>
+    <t>C3-H2</t>
+  </si>
+  <si>
+    <t>H2-H3</t>
+  </si>
+  <si>
+    <t>H3-C4</t>
+  </si>
+  <si>
+    <t>C4-C5</t>
+  </si>
+  <si>
+    <t>C5-C6</t>
+  </si>
+  <si>
+    <t>C6-C7</t>
+  </si>
+  <si>
+    <t>C7-C8</t>
+  </si>
+  <si>
+    <t>C8-C9</t>
+  </si>
+  <si>
+    <t>C9-M6</t>
+  </si>
+  <si>
+    <t>M6-H4</t>
+  </si>
+  <si>
+    <t>H4-C10</t>
+  </si>
+  <si>
+    <t>C10-C11</t>
+  </si>
+  <si>
+    <t>C11-C12</t>
+  </si>
+  <si>
+    <t>C12-C13</t>
+  </si>
+  <si>
+    <t>C13-C14</t>
+  </si>
+  <si>
+    <t>euclidean.distance.metres</t>
   </si>
 </sst>
 </file>
@@ -474,7 +567,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -497,11 +590,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -558,6 +662,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -576,7 +686,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -864,7 +974,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -874,11 +984,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB97E4CB-EAC5-A646-BEC3-C9E17C7337B6}">
   <dimension ref="A1:AG31"/>
   <sheetViews>
-    <sheetView zoomScale="174" zoomScaleNormal="162" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B16" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="174" zoomScaleNormal="162" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AC32" sqref="AC32"/>
+      <selection pane="bottomRight" activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -932,7 +1042,7 @@
         <v>8</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O1" s="3" t="s">
         <v>9</v>
@@ -953,43 +1063,43 @@
         <v>88</v>
       </c>
       <c r="U1" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="V1" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AG1" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="AG1" s="2" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.2">
@@ -3971,7 +4081,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5381714B-05BA-204C-BC88-34B6CCB1BFF8}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G22" sqref="G22"/>
     </sheetView>
@@ -3989,13 +4099,13 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -4606,14 +4716,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{191690F3-C00A-624F-AD30-A957AF041456}">
-  <dimension ref="B2:K10"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="3" max="3" width="23.6640625" customWidth="1"/>
     <col min="4" max="4" width="14.6640625" customWidth="1"/>
     <col min="6" max="6" width="12.83203125" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
@@ -4622,292 +4733,406 @@
     <col min="11" max="11" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" ht="27" x14ac:dyDescent="0.2">
-      <c r="B2" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" s="2" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="B2" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" s="5">
+        <v>19120</v>
+      </c>
+      <c r="D2" s="8"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" s="5">
+        <v>40360</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C4" s="5">
+        <v>2380</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="B5" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C5" s="5">
+        <v>39190</v>
+      </c>
+      <c r="D5" s="9"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C6" s="5">
+        <v>3520</v>
+      </c>
+      <c r="D6" s="12"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="13"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7">
         <v>6</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="B7" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C7" s="5">
+        <v>13640</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8">
         <v>7</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="B8" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C8" s="6">
+        <v>8540</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9">
         <v>8</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="B9" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C9" s="7">
+        <v>3760</v>
+      </c>
+      <c r="D9" s="9"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10">
         <v>9</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="B10" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C10" s="7">
+        <v>5670</v>
+      </c>
+      <c r="D10" s="12"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11">
         <v>10</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="B11" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="C11" s="25">
+        <v>8070</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12">
         <v>11</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B3" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" s="5" t="s">
+      <c r="B12" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="C12" s="25">
+        <v>21820</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="C13" s="25">
+        <v>8470</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14">
         <v>13</v>
       </c>
-      <c r="D3" s="9">
-        <v>106.8</v>
-      </c>
-      <c r="E3" s="6">
-        <v>13.3</v>
-      </c>
-      <c r="F3" s="5">
-        <v>3.3</v>
-      </c>
-      <c r="G3" s="5">
-        <v>12.4</v>
-      </c>
-      <c r="H3" s="11">
-        <v>28.5</v>
-      </c>
-      <c r="I3" s="6">
-        <v>53.3</v>
-      </c>
-      <c r="J3" s="6">
-        <v>4.8</v>
-      </c>
-      <c r="K3" s="6">
-        <v>3.4</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B4" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C4" s="5" t="s">
+      <c r="B14" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="C14" s="25">
+        <v>5090</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="C15" s="25">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="C16" s="25">
+        <v>13650</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="C17" s="25">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="24" t="s">
+        <v>124</v>
+      </c>
+      <c r="C18" s="25">
+        <v>10970</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="C19" s="25">
+        <v>4840</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="C20" s="25">
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21">
         <v>20</v>
       </c>
-      <c r="D4" s="9">
-        <v>2.1</v>
-      </c>
-      <c r="E4" s="6">
-        <v>7.5</v>
-      </c>
-      <c r="F4" s="5">
-        <v>0.8</v>
-      </c>
-      <c r="G4" s="5">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="H4" s="11">
-        <v>20.8</v>
-      </c>
-      <c r="I4" s="6">
-        <v>39.700000000000003</v>
-      </c>
-      <c r="J4" s="6">
-        <v>16.899999999999999</v>
-      </c>
-      <c r="K4" s="6">
-        <v>14.3</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B5" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C5" s="5" t="s">
+      <c r="B21" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="C21" s="25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="C22" s="25">
+        <v>11410</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="C23" s="25">
+        <v>5500</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24">
         <v>23</v>
       </c>
-      <c r="D5" s="9">
-        <v>0.4</v>
-      </c>
-      <c r="E5" s="6">
-        <v>6.3</v>
-      </c>
-      <c r="F5" s="5">
-        <v>20.6</v>
-      </c>
-      <c r="G5" s="5">
-        <v>0</v>
-      </c>
-      <c r="H5" s="11">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="I5" s="6">
-        <v>55.3</v>
-      </c>
-      <c r="J5" s="6">
-        <v>19.399999999999999</v>
-      </c>
-      <c r="K5" s="6">
-        <v>12.7</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B6" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="12">
-        <v>1.5</v>
-      </c>
-      <c r="E6" s="13">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="F6" s="14">
-        <v>2.1</v>
-      </c>
-      <c r="G6" s="5">
-        <v>8.1</v>
-      </c>
-      <c r="H6" s="15">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="I6" s="6">
-        <v>39.700000000000003</v>
-      </c>
-      <c r="J6" s="6">
-        <v>15.9</v>
-      </c>
-      <c r="K6" s="13">
-        <v>17.899999999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B7" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="9">
-        <v>1.2</v>
-      </c>
-      <c r="E7" s="6">
-        <v>13.1</v>
-      </c>
-      <c r="F7" s="14">
-        <v>10</v>
-      </c>
-      <c r="G7" s="5">
-        <v>0</v>
-      </c>
-      <c r="H7" s="15">
-        <v>8</v>
-      </c>
-      <c r="I7" s="6">
-        <v>64.400000000000006</v>
-      </c>
-      <c r="J7" s="6">
-        <v>14.4</v>
-      </c>
-      <c r="K7" s="6">
-        <v>9.9</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B8" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="9">
-        <v>1.7</v>
-      </c>
-      <c r="E8" s="6">
-        <v>13.1</v>
-      </c>
-      <c r="F8" s="5">
-        <v>0.6</v>
-      </c>
-      <c r="G8" s="5">
-        <v>1.2</v>
-      </c>
-      <c r="H8" s="11">
-        <v>66.8</v>
-      </c>
-      <c r="I8" s="6">
-        <v>20.7</v>
-      </c>
-      <c r="J8" s="6">
-        <v>0</v>
-      </c>
-      <c r="K8" s="6">
-        <v>6.7</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B9" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="9">
-        <v>11.6</v>
-      </c>
-      <c r="E9" s="6">
-        <v>14.3</v>
-      </c>
-      <c r="F9" s="5">
-        <v>1.7</v>
-      </c>
-      <c r="G9" s="14">
-        <v>3.9</v>
-      </c>
-      <c r="H9" s="15">
-        <v>68.8</v>
-      </c>
-      <c r="I9" s="6">
-        <v>22.8</v>
-      </c>
-      <c r="J9" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="K9" s="6">
-        <v>2.7</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B10" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="12">
-        <v>14.2</v>
-      </c>
-      <c r="E10" s="6">
-        <v>10.7</v>
-      </c>
-      <c r="F10" s="5">
-        <v>5.3</v>
-      </c>
-      <c r="G10" s="5">
-        <v>4.2</v>
-      </c>
-      <c r="H10" s="11">
-        <v>78.3</v>
-      </c>
-      <c r="I10" s="6">
-        <v>15.2</v>
-      </c>
-      <c r="J10" s="6">
-        <v>0.51</v>
-      </c>
-      <c r="K10" s="6">
-        <v>0.3</v>
+      <c r="B24" s="24" t="s">
+        <v>130</v>
+      </c>
+      <c r="C24" s="25">
+        <v>5350</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="C25" s="25">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="C26" s="25">
+        <v>12740</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="C27" s="25">
+        <v>1610</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="C28" s="25">
+        <v>2430</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="C29" s="25">
+        <v>21430</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" s="24" t="s">
+        <v>136</v>
+      </c>
+      <c r="C30" s="25">
+        <v>15960</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
upd - adjusted excel table sheet 3; added new script for site distance/doc correlation.
</commit_message>
<xml_diff>
--- a/Watershed_table_v1.xlsx
+++ b/Watershed_table_v1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Matt 1/Desktop/2020 Trent University/R/Thesis Data/MSc_data_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1651C69-EAC3-734F-801B-8E6FA57DAAD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5F25153-DC1B-C142-BD7C-71615592B943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1820" yWindow="1740" windowWidth="27500" windowHeight="17500" xr2:uid="{3AD1715B-176F-3140-B9AE-F64F14EE2DEE}"/>
+    <workbookView xWindow="9120" yWindow="500" windowWidth="27500" windowHeight="17500" activeTab="2" xr2:uid="{3AD1715B-176F-3140-B9AE-F64F14EE2DEE}"/>
   </bookViews>
   <sheets>
     <sheet name="Master_watershed_table_v1.00" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="137">
   <si>
     <t>Site name</t>
   </si>
@@ -381,9 +381,6 @@
   </si>
   <si>
     <t>Coefficient of Variation</t>
-  </si>
-  <si>
-    <t>pair</t>
   </si>
   <si>
     <t>site.pair</t>
@@ -984,8 +981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB97E4CB-EAC5-A646-BEC3-C9E17C7337B6}">
   <dimension ref="A1:AG31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="174" zoomScaleNormal="162" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="174" zoomScaleNormal="162" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="G20" sqref="G20"/>
@@ -4716,422 +4713,333 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{191690F3-C00A-624F-AD30-A957AF041456}">
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="23.6640625" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" customWidth="1"/>
-    <col min="6" max="6" width="12.83203125" customWidth="1"/>
-    <col min="8" max="8" width="14" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" customWidth="1"/>
-    <col min="10" max="10" width="14" customWidth="1"/>
-    <col min="11" max="11" width="11.6640625" customWidth="1"/>
+    <col min="2" max="2" width="21.83203125" customWidth="1"/>
+    <col min="4" max="4" width="23.6640625" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" customWidth="1"/>
+    <col min="9" max="9" width="14" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" customWidth="1"/>
+    <col min="11" max="11" width="14" customWidth="1"/>
+    <col min="12" max="12" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>106</v>
       </c>
       <c r="B1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="C1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C2" s="5">
+      <c r="B2" s="5">
         <v>19120</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="3"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="2"/>
       <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="3"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="C3" s="5">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B3" s="5">
         <v>40360</v>
       </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="6"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="5"/>
       <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="6"/>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="C4" s="5">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B4" s="5">
         <v>2380</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="6"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="5"/>
       <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="C5" s="5">
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B5" s="5">
         <v>39190</v>
       </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="6"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="5"/>
       <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="6"/>
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" s="4" t="s">
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B6" s="5">
+        <v>3520</v>
+      </c>
+      <c r="C6" s="12"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="13"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="C6" s="5">
-        <v>3520</v>
-      </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="13"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="C7" s="5">
+      <c r="B7" s="5">
         <v>13640</v>
       </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="15"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="6"/>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C8" s="6">
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B8" s="6">
         <v>8540</v>
       </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="6"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="5"/>
       <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="6"/>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C9" s="7">
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B9" s="7">
         <v>3760</v>
       </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="15"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="6"/>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C10" s="7">
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B10" s="7">
         <v>5670</v>
       </c>
-      <c r="D10" s="12"/>
-      <c r="E10" s="6"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="5"/>
       <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="6"/>
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" s="24" t="s">
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="B11" s="25">
+        <v>8070</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="C11" s="25">
-        <v>8070</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="25">
+        <v>21820</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="24" t="s">
         <v>118</v>
       </c>
-      <c r="C12" s="25">
-        <v>21820</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="25">
+        <v>8470</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="C13" s="25">
-        <v>8470</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" s="24" t="s">
+      <c r="B14" s="25">
+        <v>5090</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="24" t="s">
         <v>120</v>
       </c>
-      <c r="C14" s="25">
-        <v>5090</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="25">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="24" t="s">
         <v>121</v>
       </c>
-      <c r="C15" s="25">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" s="24" t="s">
+      <c r="B16" s="25">
+        <v>13650</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="24" t="s">
         <v>122</v>
       </c>
-      <c r="C16" s="25">
-        <v>13650</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="25">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="C17" s="25">
-        <v>709</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" s="24" t="s">
+      <c r="B18" s="25">
+        <v>10970</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="C18" s="25">
-        <v>10970</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" s="24" t="s">
+      <c r="B19" s="25">
+        <v>4840</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="24" t="s">
         <v>125</v>
       </c>
-      <c r="C19" s="25">
-        <v>4840</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" s="24" t="s">
+      <c r="B20" s="25">
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="24" t="s">
         <v>126</v>
       </c>
-      <c r="C20" s="25">
-        <v>5400</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21" s="24" t="s">
+      <c r="B21" s="25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="C21" s="25">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="B22" s="24" t="s">
+      <c r="B22" s="25">
+        <v>11410</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="24" t="s">
         <v>128</v>
       </c>
-      <c r="C22" s="25">
-        <v>11410</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>22</v>
-      </c>
-      <c r="B23" s="24" t="s">
+      <c r="B23" s="25">
+        <v>5500</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="24" t="s">
         <v>129</v>
       </c>
-      <c r="C23" s="25">
-        <v>5500</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>23</v>
-      </c>
-      <c r="B24" s="24" t="s">
+      <c r="B24" s="25">
+        <v>5350</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="C24" s="25">
-        <v>5350</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>24</v>
-      </c>
-      <c r="B25" s="24" t="s">
+      <c r="B25" s="25">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="C25" s="25">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>25</v>
-      </c>
-      <c r="B26" s="24" t="s">
+      <c r="B26" s="25">
+        <v>12740</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="C26" s="25">
-        <v>12740</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>26</v>
-      </c>
-      <c r="B27" s="24" t="s">
+      <c r="B27" s="25">
+        <v>1610</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="24" t="s">
         <v>133</v>
       </c>
-      <c r="C27" s="25">
-        <v>1610</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>27</v>
-      </c>
-      <c r="B28" s="24" t="s">
+      <c r="B28" s="25">
+        <v>2430</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="24" t="s">
         <v>134</v>
       </c>
-      <c r="C28" s="25">
-        <v>2430</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>28</v>
-      </c>
-      <c r="B29" s="24" t="s">
+      <c r="B29" s="25">
+        <v>21430</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="24" t="s">
         <v>135</v>
       </c>
-      <c r="C29" s="25">
-        <v>21430</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>29</v>
-      </c>
-      <c r="B30" s="24" t="s">
-        <v>136</v>
-      </c>
-      <c r="C30" s="25">
+      <c r="B30" s="25">
         <v>15960</v>
       </c>
     </row>

</xml_diff>

<commit_message>
upd - large upd, graphs for committee meeting; new master DOC table for use with heirarchical partitioning.
</commit_message>
<xml_diff>
--- a/Watershed_table_v1.xlsx
+++ b/Watershed_table_v1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Matt 1/Desktop/2020 Trent University/R/Thesis Data/MSc_data_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A560505C-B0C6-F540-BCD4-3805EFAF4533}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80B78E54-306A-6F45-9E24-F070D5571D7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1300" yWindow="500" windowWidth="27500" windowHeight="17500" xr2:uid="{3AD1715B-176F-3140-B9AE-F64F14EE2DEE}"/>
+    <workbookView xWindow="18660" yWindow="3420" windowWidth="27500" windowHeight="17500" xr2:uid="{3AD1715B-176F-3140-B9AE-F64F14EE2DEE}"/>
   </bookViews>
   <sheets>
     <sheet name="Master_watershed_table_v1.00" sheetId="1" r:id="rId1"/>
@@ -844,7 +844,7 @@
   <dimension ref="A1:AF31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="174" zoomScaleNormal="162" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="P1" sqref="P1:P1048576"/>

</xml_diff>

<commit_message>
upd - DOC, flux, SUVA base model mreg plot
</commit_message>
<xml_diff>
--- a/Watershed_table_v1.xlsx
+++ b/Watershed_table_v1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Matt 1/Desktop/2020 Trent University/R/Thesis Data/MSc_data_analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Matt 1/Desktop/MSc/R/thesis_data/MSc_data_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80B78E54-306A-6F45-9E24-F070D5571D7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1F8E915-67B5-B345-9DCE-FE8DF66ABC09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18660" yWindow="3420" windowWidth="27500" windowHeight="17500" xr2:uid="{3AD1715B-176F-3140-B9AE-F64F14EE2DEE}"/>
+    <workbookView xWindow="18680" yWindow="500" windowWidth="19720" windowHeight="20420" xr2:uid="{3AD1715B-176F-3140-B9AE-F64F14EE2DEE}"/>
   </bookViews>
   <sheets>
     <sheet name="Master_watershed_table_v1.00" sheetId="1" r:id="rId1"/>
@@ -847,7 +847,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P1" sqref="P1:P1048576"/>
+      <selection pane="bottomRight" activeCell="A31" sqref="A31:XFD31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>